<commit_message>
image array splited with comma
</commit_message>
<xml_diff>
--- a/ChaoKaiQiProducts.xlsx
+++ b/ChaoKaiQiProducts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12210"/>
+    <workbookView windowWidth="21945" windowHeight="9720"/>
   </bookViews>
   <sheets>
     <sheet name="Snap rotate style" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="221">
   <si>
     <t>Cover Name</t>
   </si>
@@ -78,7 +78,7 @@
     <t>/ProductImages/snapRotationStyle/snapRotationStyle (1)</t>
   </si>
   <si>
-    <t>/ProductImages/snapRotationStyle/snapRotationStyle (1),/ProductImages/snapRotationStyle/snapRotationStyle (2), /ProductImages/snapRotationStyle/snapRotationStyle (3), /ProductImages/snapRotationStyle/snapRotationStyle (4), /ProductImages/snapRotationStyle/snapRotationStyle (5), /ProductImages/snapRotationStyle/snapRotationStyle (6), /ProductImages/snapRotationStyle/snapRotationStyle (7), /ProductImages/snapRotationStyle/snapRotationStyle (8), /ProductImages/snapRotationStyle/colors/babyPink,/ProductImages/snapRotationStyle/colors/black,/ProductImages/snapRotationStyle/colors/deepGreen,/ProductImages/snapRotationStyle/colors/gray,/ProductImages/snapRotationStyle/colors/lavanderPurple,/ProductImages/snapRotationStyle/colors/whiteIce,</t>
+    <t>/ProductImages/snapRotationStyle/snapRotationStyle (1),/ProductImages/snapRotationStyle/snapRotationStyle (2), /ProductImages/snapRotationStyle/snapRotationStyle (3), /ProductImages/snapRotationStyle/snapRotationStyle (4), /ProductImages/snapRotationStyle/snapRotationStyle (5), /ProductImages/snapRotationStyle/snapRotationStyle (6), /ProductImages/snapRotationStyle/snapRotationStyle (7), /ProductImages/snapRotationStyle/snapRotationStyle (8), /ProductImages/snapRotationStyle/colors/babyPink,/ProductImages/snapRotationStyle/colors/black,/ProductImages/snapRotationStyle/colors/deepGreen,/ProductImages/snapRotationStyle/colors/gray,/ProductImages/snapRotationStyle/colors/lavanderPurple,/ProductImages/snapRotationStyle/colors/whiteIce</t>
   </si>
   <si>
     <t>Snap Rotation Style</t>
@@ -93,36 +93,24 @@
     <t>/ProductImages/snapRotationStyle/snapRotationStyle (2)</t>
   </si>
   <si>
-    <t>/ProductImages/snapRotationStyle/snapRotationStyle (1),/ProductImages/snapRotationStyle/snapRotationStyle (2), /ProductImages/snapRotationStyle/snapRotationStyle (3), /ProductImages/snapRotationStyle/snapRotationStyle (4), /ProductImages/snapRotationStyle/snapRotationStyle (5), /ProductImages/snapRotationStyle/snapRotationStyle (6), /ProductImages/snapRotationStyle/snapRotationStyle (7), /ProductImages/snapRotationStyle/snapRotationStyle (9), /ProductImages/snapRotationStyle/colors/babyPink,/ProductImages/snapRotationStyle/colors/black,/ProductImages/snapRotationStyle/colors/deepGreen,/ProductImages/snapRotationStyle/colors/gray,/ProductImages/snapRotationStyle/colors/lavanderPurple,/ProductImages/snapRotationStyle/colors/whiteIce,</t>
-  </si>
-  <si>
     <t>iPad 9.7 2018</t>
   </si>
   <si>
     <t>/ProductImages/snapRotationStyle/snapRotationStyle (3)</t>
   </si>
   <si>
-    <t>/ProductImages/snapRotationStyle/snapRotationStyle (1),/ProductImages/snapRotationStyle/snapRotationStyle (2), /ProductImages/snapRotationStyle/snapRotationStyle (3), /ProductImages/snapRotationStyle/snapRotationStyle (4), /ProductImages/snapRotationStyle/snapRotationStyle (5), /ProductImages/snapRotationStyle/snapRotationStyle (6), /ProductImages/snapRotationStyle/snapRotationStyle (7), /ProductImages/snapRotationStyle/snapRotationStyle (10), /ProductImages/snapRotationStyle/colors/babyPink,/ProductImages/snapRotationStyle/colors/black,/ProductImages/snapRotationStyle/colors/deepGreen,/ProductImages/snapRotationStyle/colors/gray,/ProductImages/snapRotationStyle/colors/lavanderPurple,/ProductImages/snapRotationStyle/colors/whiteIce,</t>
-  </si>
-  <si>
     <t>iPad 9.7 Air1</t>
   </si>
   <si>
     <t>/ProductImages/snapRotationStyle/snapRotationStyle (4)</t>
   </si>
   <si>
-    <t>/ProductImages/snapRotationStyle/snapRotationStyle (1),/ProductImages/snapRotationStyle/snapRotationStyle (2), /ProductImages/snapRotationStyle/snapRotationStyle (3), /ProductImages/snapRotationStyle/snapRotationStyle (4), /ProductImages/snapRotationStyle/snapRotationStyle (5), /ProductImages/snapRotationStyle/snapRotationStyle (6), /ProductImages/snapRotationStyle/snapRotationStyle (7), /ProductImages/snapRotationStyle/snapRotationStyle (11), /ProductImages/snapRotationStyle/colors/babyPink,/ProductImages/snapRotationStyle/colors/black,/ProductImages/snapRotationStyle/colors/deepGreen,/ProductImages/snapRotationStyle/colors/gray,/ProductImages/snapRotationStyle/colors/lavanderPurple,/ProductImages/snapRotationStyle/colors/whiteIce,</t>
-  </si>
-  <si>
     <t>iPad 9.7 Air2</t>
   </si>
   <si>
     <t>/ProductImages/snapRotationStyle/snapRotationStyle (5)</t>
   </si>
   <si>
-    <t>/ProductImages/snapRotationStyle/snapRotationStyle (1),/ProductImages/snapRotationStyle/snapRotationStyle (2), /ProductImages/snapRotationStyle/snapRotationStyle (3), /ProductImages/snapRotationStyle/snapRotationStyle (4), /ProductImages/snapRotationStyle/snapRotationStyle (5), /ProductImages/snapRotationStyle/snapRotationStyle (6), /ProductImages/snapRotationStyle/snapRotationStyle (7), /ProductImages/snapRotationStyle/snapRotationStyle (12), /ProductImages/snapRotationStyle/colors/babyPink,/ProductImages/snapRotationStyle/colors/black,/ProductImages/snapRotationStyle/colors/deepGreen,/ProductImages/snapRotationStyle/colors/gray,/ProductImages/snapRotationStyle/colors/lavanderPurple,/ProductImages/snapRotationStyle/colors/whiteIce,</t>
-  </si>
-  <si>
     <t>iPad 10.2 2019</t>
   </si>
   <si>
@@ -132,82 +120,49 @@
     <t>/ProductImages/snapRotationStyle/snapRotationStyle (6)</t>
   </si>
   <si>
-    <t>/ProductImages/snapRotationStyle/snapRotationStyle (1),/ProductImages/snapRotationStyle/snapRotationStyle (2), /ProductImages/snapRotationStyle/snapRotationStyle (3), /ProductImages/snapRotationStyle/snapRotationStyle (4), /ProductImages/snapRotationStyle/snapRotationStyle (5), /ProductImages/snapRotationStyle/snapRotationStyle (6), /ProductImages/snapRotationStyle/snapRotationStyle (7), /ProductImages/snapRotationStyle/snapRotationStyle (13), /ProductImages/snapRotationStyle/colors/babyPink,/ProductImages/snapRotationStyle/colors/black,/ProductImages/snapRotationStyle/colors/deepGreen,/ProductImages/snapRotationStyle/colors/gray,/ProductImages/snapRotationStyle/colors/lavanderPurple,/ProductImages/snapRotationStyle/colors/whiteIce,</t>
-  </si>
-  <si>
     <t>iPad 10.2 2020</t>
   </si>
   <si>
     <t>/ProductImages/snapRotationStyle/snapRotationStyle (7)</t>
   </si>
   <si>
-    <t>/ProductImages/snapRotationStyle/snapRotationStyle (1),/ProductImages/snapRotationStyle/snapRotationStyle (2), /ProductImages/snapRotationStyle/snapRotationStyle (3), /ProductImages/snapRotationStyle/snapRotationStyle (4), /ProductImages/snapRotationStyle/snapRotationStyle (5), /ProductImages/snapRotationStyle/snapRotationStyle (6), /ProductImages/snapRotationStyle/snapRotationStyle (7), /ProductImages/snapRotationStyle/snapRotationStyle (14), /ProductImages/snapRotationStyle/colors/babyPink,/ProductImages/snapRotationStyle/colors/black,/ProductImages/snapRotationStyle/colors/deepGreen,/ProductImages/snapRotationStyle/colors/gray,/ProductImages/snapRotationStyle/colors/lavanderPurple,/ProductImages/snapRotationStyle/colors/whiteIce,</t>
-  </si>
-  <si>
     <t>iPad 10.2 2021</t>
   </si>
   <si>
     <t>/ProductImages/snapRotationStyle/snapRotationStyle (8)</t>
   </si>
   <si>
-    <t>/ProductImages/snapRotationStyle/snapRotationStyle (1),/ProductImages/snapRotationStyle/snapRotationStyle (2), /ProductImages/snapRotationStyle/snapRotationStyle (3), /ProductImages/snapRotationStyle/snapRotationStyle (4), /ProductImages/snapRotationStyle/snapRotationStyle (5), /ProductImages/snapRotationStyle/snapRotationStyle (6), /ProductImages/snapRotationStyle/snapRotationStyle (7), /ProductImages/snapRotationStyle/snapRotationStyle (15), /ProductImages/snapRotationStyle/colors/babyPink,/ProductImages/snapRotationStyle/colors/black,/ProductImages/snapRotationStyle/colors/deepGreen,/ProductImages/snapRotationStyle/colors/gray,/ProductImages/snapRotationStyle/colors/lavanderPurple,/ProductImages/snapRotationStyle/colors/whiteIce,</t>
-  </si>
-  <si>
     <t>iPad 10.9 2022</t>
   </si>
   <si>
     <t>254 * 192 * 13</t>
   </si>
   <si>
-    <t>/ProductImages/snapRotationStyle/snapRotationStyle (1),/ProductImages/snapRotationStyle/snapRotationStyle (2), /ProductImages/snapRotationStyle/snapRotationStyle (3), /ProductImages/snapRotationStyle/snapRotationStyle (4), /ProductImages/snapRotationStyle/snapRotationStyle (5), /ProductImages/snapRotationStyle/snapRotationStyle (6), /ProductImages/snapRotationStyle/snapRotationStyle (7), /ProductImages/snapRotationStyle/snapRotationStyle (16), /ProductImages/snapRotationStyle/colors/babyPink,/ProductImages/snapRotationStyle/colors/black,/ProductImages/snapRotationStyle/colors/deepGreen,/ProductImages/snapRotationStyle/colors/gray,/ProductImages/snapRotationStyle/colors/lavanderPurple,/ProductImages/snapRotationStyle/colors/whiteIce,</t>
-  </si>
-  <si>
     <t>ipad Pro 11</t>
   </si>
   <si>
     <t>253 * 194 * 14</t>
   </si>
   <si>
-    <t>/ProductImages/snapRotationStyle/snapRotationStyle (1),/ProductImages/snapRotationStyle/snapRotationStyle (2), /ProductImages/snapRotationStyle/snapRotationStyle (3), /ProductImages/snapRotationStyle/snapRotationStyle (4), /ProductImages/snapRotationStyle/snapRotationStyle (5), /ProductImages/snapRotationStyle/snapRotationStyle (6), /ProductImages/snapRotationStyle/snapRotationStyle (7), /ProductImages/snapRotationStyle/snapRotationStyle (17), /ProductImages/snapRotationStyle/colors/babyPink,/ProductImages/snapRotationStyle/colors/black,/ProductImages/snapRotationStyle/colors/deepGreen,/ProductImages/snapRotationStyle/colors/gray,/ProductImages/snapRotationStyle/colors/lavanderPurple,/ProductImages/snapRotationStyle/colors/whiteIce,</t>
-  </si>
-  <si>
     <t>ipad Air4</t>
   </si>
   <si>
-    <t>/ProductImages/snapRotationStyle/snapRotationStyle (1),/ProductImages/snapRotationStyle/snapRotationStyle (2), /ProductImages/snapRotationStyle/snapRotationStyle (3), /ProductImages/snapRotationStyle/snapRotationStyle (4), /ProductImages/snapRotationStyle/snapRotationStyle (5), /ProductImages/snapRotationStyle/snapRotationStyle (6), /ProductImages/snapRotationStyle/snapRotationStyle (7), /ProductImages/snapRotationStyle/snapRotationStyle (18), /ProductImages/snapRotationStyle/colors/babyPink,/ProductImages/snapRotationStyle/colors/black,/ProductImages/snapRotationStyle/colors/deepGreen,/ProductImages/snapRotationStyle/colors/gray,/ProductImages/snapRotationStyle/colors/lavanderPurple,/ProductImages/snapRotationStyle/colors/whiteIce,</t>
-  </si>
-  <si>
     <t>ipad Air5</t>
   </si>
   <si>
-    <t>/ProductImages/snapRotationStyle/snapRotationStyle (1),/ProductImages/snapRotationStyle/snapRotationStyle (2), /ProductImages/snapRotationStyle/snapRotationStyle (3), /ProductImages/snapRotationStyle/snapRotationStyle (4), /ProductImages/snapRotationStyle/snapRotationStyle (5), /ProductImages/snapRotationStyle/snapRotationStyle (6), /ProductImages/snapRotationStyle/snapRotationStyle (7), /ProductImages/snapRotationStyle/snapRotationStyle (19), /ProductImages/snapRotationStyle/colors/babyPink,/ProductImages/snapRotationStyle/colors/black,/ProductImages/snapRotationStyle/colors/deepGreen,/ProductImages/snapRotationStyle/colors/gray,/ProductImages/snapRotationStyle/colors/lavanderPurple,/ProductImages/snapRotationStyle/colors/whiteIce,</t>
-  </si>
-  <si>
     <t>ipad Pro 12.9 2018</t>
   </si>
   <si>
     <t>285 * 230 * 15</t>
   </si>
   <si>
-    <t>/ProductImages/snapRotationStyle/snapRotationStyle (1),/ProductImages/snapRotationStyle/snapRotationStyle (2), /ProductImages/snapRotationStyle/snapRotationStyle (3), /ProductImages/snapRotationStyle/snapRotationStyle (4), /ProductImages/snapRotationStyle/snapRotationStyle (5), /ProductImages/snapRotationStyle/snapRotationStyle (6), /ProductImages/snapRotationStyle/snapRotationStyle (7), /ProductImages/snapRotationStyle/snapRotationStyle (20), /ProductImages/snapRotationStyle/colors/babyPink,/ProductImages/snapRotationStyle/colors/black,/ProductImages/snapRotationStyle/colors/deepGreen,/ProductImages/snapRotationStyle/colors/gray,/ProductImages/snapRotationStyle/colors/lavanderPurple,/ProductImages/snapRotationStyle/colors/whiteIce,</t>
-  </si>
-  <si>
     <t>ipad Pro 12.9 2020</t>
   </si>
   <si>
-    <t>/ProductImages/snapRotationStyle/snapRotationStyle (1),/ProductImages/snapRotationStyle/snapRotationStyle (2), /ProductImages/snapRotationStyle/snapRotationStyle (3), /ProductImages/snapRotationStyle/snapRotationStyle (4), /ProductImages/snapRotationStyle/snapRotationStyle (5), /ProductImages/snapRotationStyle/snapRotationStyle (6), /ProductImages/snapRotationStyle/snapRotationStyle (7), /ProductImages/snapRotationStyle/snapRotationStyle (21), /ProductImages/snapRotationStyle/colors/babyPink,/ProductImages/snapRotationStyle/colors/black,/ProductImages/snapRotationStyle/colors/deepGreen,/ProductImages/snapRotationStyle/colors/gray,/ProductImages/snapRotationStyle/colors/lavanderPurple,/ProductImages/snapRotationStyle/colors/whiteIce,</t>
-  </si>
-  <si>
     <t>ipad Pro 12.9 2021</t>
   </si>
   <si>
-    <t>/ProductImages/snapRotationStyle/snapRotationStyle (1),/ProductImages/snapRotationStyle/snapRotationStyle (2), /ProductImages/snapRotationStyle/snapRotationStyle (3), /ProductImages/snapRotationStyle/snapRotationStyle (4), /ProductImages/snapRotationStyle/snapRotationStyle (5), /ProductImages/snapRotationStyle/snapRotationStyle (6), /ProductImages/snapRotationStyle/snapRotationStyle (7), /ProductImages/snapRotationStyle/snapRotationStyle (22), /ProductImages/snapRotationStyle/colors/babyPink,/ProductImages/snapRotationStyle/colors/black,/ProductImages/snapRotationStyle/colors/deepGreen,/ProductImages/snapRotationStyle/colors/gray,/ProductImages/snapRotationStyle/colors/lavanderPurple,/ProductImages/snapRotationStyle/colors/whiteIce,</t>
-  </si>
-  <si>
     <t>ipad Pro 12.9 2022</t>
-  </si>
-  <si>
-    <t>/ProductImages/snapRotationStyle/snapRotationStyle (1),/ProductImages/snapRotationStyle/snapRotationStyle (2), /ProductImages/snapRotationStyle/snapRotationStyle (3), /ProductImages/snapRotationStyle/snapRotationStyle (4), /ProductImages/snapRotationStyle/snapRotationStyle (5), /ProductImages/snapRotationStyle/snapRotationStyle (6), /ProductImages/snapRotationStyle/snapRotationStyle (7), /ProductImages/snapRotationStyle/snapRotationStyle (23), /ProductImages/snapRotationStyle/colors/babyPink,/ProductImages/snapRotationStyle/colors/black,/ProductImages/snapRotationStyle/colors/deepGreen,/ProductImages/snapRotationStyle/colors/gray,/ProductImages/snapRotationStyle/colors/lavanderPurple,/ProductImages/snapRotationStyle/colors/whiteIce,</t>
   </si>
   <si>
     <t>Snap Closure Full Package</t>
@@ -2570,8 +2525,8 @@
   <sheetPr/>
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -2679,7 +2634,7 @@
         <v>20</v>
       </c>
       <c r="J3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -2687,7 +2642,7 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
@@ -2702,10 +2657,10 @@
         <v>231</v>
       </c>
       <c r="I4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J4" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -2713,7 +2668,7 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
@@ -2728,10 +2683,10 @@
         <v>231</v>
       </c>
       <c r="I5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J5" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -2739,7 +2694,7 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>
@@ -2754,10 +2709,10 @@
         <v>231</v>
       </c>
       <c r="I6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J6" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -2765,7 +2720,7 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
@@ -2774,16 +2729,16 @@
         <v>2.8</v>
       </c>
       <c r="G7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H7">
         <v>245</v>
       </c>
       <c r="I7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J7" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -2791,7 +2746,7 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
         <v>13</v>
@@ -2800,16 +2755,16 @@
         <v>2.8</v>
       </c>
       <c r="G8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H8">
         <v>245</v>
       </c>
       <c r="I8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="J8" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2817,7 +2772,7 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
         <v>13</v>
@@ -2826,16 +2781,16 @@
         <v>2.8</v>
       </c>
       <c r="G9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H9">
         <v>245</v>
       </c>
       <c r="I9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="J9" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -2843,7 +2798,7 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
         <v>13</v>
@@ -2852,7 +2807,7 @@
         <v>2.8</v>
       </c>
       <c r="G10" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="H10">
         <v>250</v>
@@ -2861,7 +2816,7 @@
         <v>15</v>
       </c>
       <c r="J10" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -2869,7 +2824,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -2878,7 +2833,7 @@
         <v>2.8</v>
       </c>
       <c r="G11" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="H11">
         <v>251</v>
@@ -2887,7 +2842,7 @@
         <v>20</v>
       </c>
       <c r="J11" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -2895,7 +2850,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
         <v>13</v>
@@ -2904,16 +2859,16 @@
         <v>2.8</v>
       </c>
       <c r="G12" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="H12">
         <v>251</v>
       </c>
       <c r="I12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J12" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -2921,7 +2876,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s">
         <v>13</v>
@@ -2930,16 +2885,16 @@
         <v>2.8</v>
       </c>
       <c r="G13" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="H13">
         <v>251</v>
       </c>
       <c r="I13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J13" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -2947,7 +2902,7 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D14" t="s">
         <v>13</v>
@@ -2956,16 +2911,16 @@
         <v>4.2</v>
       </c>
       <c r="G14" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="H14">
         <v>490</v>
       </c>
       <c r="I14" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J14" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -2973,7 +2928,7 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D15" t="s">
         <v>13</v>
@@ -2982,16 +2937,16 @@
         <v>4.2</v>
       </c>
       <c r="G15" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="H15">
         <v>490</v>
       </c>
       <c r="I15" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J15" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -2999,7 +2954,7 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="D16" t="s">
         <v>13</v>
@@ -3008,16 +2963,16 @@
         <v>4.2</v>
       </c>
       <c r="G16" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="H16">
         <v>490</v>
       </c>
       <c r="I16" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="J16" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -3025,7 +2980,7 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="D17" t="s">
         <v>13</v>
@@ -3034,16 +2989,16 @@
         <v>4.2</v>
       </c>
       <c r="G17" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="H17">
         <v>490</v>
       </c>
       <c r="I17" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="J17" t="s">
-        <v>59</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -3119,7 +3074,7 @@
     </row>
     <row r="2" customFormat="1" spans="1:8">
       <c r="A2" s="9" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>12</v>
@@ -3131,7 +3086,7 @@
         <v>3.1</v>
       </c>
       <c r="G2" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="H2">
         <v>259</v>
@@ -3139,7 +3094,7 @@
     </row>
     <row r="3" customFormat="1" spans="1:8">
       <c r="A3" s="9" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
@@ -3151,7 +3106,7 @@
         <v>3.5</v>
       </c>
       <c r="G3" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="H3">
         <v>368</v>
@@ -3159,10 +3114,10 @@
     </row>
     <row r="4" customFormat="1" spans="1:8">
       <c r="A4" s="9" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
@@ -3171,7 +3126,7 @@
         <v>3.5</v>
       </c>
       <c r="G4" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="H4">
         <v>368</v>
@@ -3179,10 +3134,10 @@
     </row>
     <row r="5" customFormat="1" spans="1:8">
       <c r="A5" s="9" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
@@ -3191,7 +3146,7 @@
         <v>3.5</v>
       </c>
       <c r="G5" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="H5">
         <v>368</v>
@@ -3199,10 +3154,10 @@
     </row>
     <row r="6" customFormat="1" spans="1:8">
       <c r="A6" s="9" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>
@@ -3211,7 +3166,7 @@
         <v>3.5</v>
       </c>
       <c r="G6" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="H6">
         <v>368</v>
@@ -3219,10 +3174,10 @@
     </row>
     <row r="7" customFormat="1" spans="1:8">
       <c r="A7" s="9" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
@@ -3231,7 +3186,7 @@
         <v>3.5</v>
       </c>
       <c r="G7" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="H7">
         <v>434</v>
@@ -3239,10 +3194,10 @@
     </row>
     <row r="8" customFormat="1" spans="1:8">
       <c r="A8" s="9" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
         <v>13</v>
@@ -3251,7 +3206,7 @@
         <v>3.5</v>
       </c>
       <c r="G8" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="H8">
         <v>434</v>
@@ -3259,10 +3214,10 @@
     </row>
     <row r="9" customFormat="1" spans="1:8">
       <c r="A9" s="9" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
         <v>13</v>
@@ -3271,7 +3226,7 @@
         <v>3.5</v>
       </c>
       <c r="G9" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="H9">
         <v>434</v>
@@ -3279,10 +3234,10 @@
     </row>
     <row r="10" customFormat="1" spans="1:8">
       <c r="A10" s="9" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
         <v>13</v>
@@ -3291,7 +3246,7 @@
         <v>3.5</v>
       </c>
       <c r="G10" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="H10">
         <v>357</v>
@@ -3299,10 +3254,10 @@
     </row>
     <row r="11" customFormat="1" spans="1:8">
       <c r="A11" s="9" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -3311,7 +3266,7 @@
         <v>3.5</v>
       </c>
       <c r="G11" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="H11">
         <v>432</v>
@@ -3319,10 +3274,10 @@
     </row>
     <row r="12" customFormat="1" spans="1:8">
       <c r="A12" s="9" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
         <v>13</v>
@@ -3331,7 +3286,7 @@
         <v>3.5</v>
       </c>
       <c r="G12" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="H12">
         <v>432</v>
@@ -3339,10 +3294,10 @@
     </row>
     <row r="13" customFormat="1" spans="1:8">
       <c r="A13" s="9" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s">
         <v>13</v>
@@ -3351,7 +3306,7 @@
         <v>3.5</v>
       </c>
       <c r="G13" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="H13">
         <v>432</v>
@@ -3359,10 +3314,10 @@
     </row>
     <row r="14" customFormat="1" spans="1:8">
       <c r="A14" s="9" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D14" t="s">
         <v>13</v>
@@ -3371,7 +3326,7 @@
         <v>4.7</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="H14">
         <v>551</v>
@@ -3379,10 +3334,10 @@
     </row>
     <row r="15" customFormat="1" spans="1:8">
       <c r="A15" s="9" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D15" t="s">
         <v>13</v>
@@ -3391,7 +3346,7 @@
         <v>4.7</v>
       </c>
       <c r="G15" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="H15">
         <v>551</v>
@@ -3399,10 +3354,10 @@
     </row>
     <row r="16" customFormat="1" spans="1:8">
       <c r="A16" s="9" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="D16" t="s">
         <v>13</v>
@@ -3411,7 +3366,7 @@
         <v>4.7</v>
       </c>
       <c r="G16" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="H16">
         <v>551</v>
@@ -3419,10 +3374,10 @@
     </row>
     <row r="17" customFormat="1" spans="1:8">
       <c r="A17" s="9" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="D17" t="s">
         <v>13</v>
@@ -3431,7 +3386,7 @@
         <v>4.7</v>
       </c>
       <c r="G17" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="H17">
         <v>551</v>
@@ -3498,7 +3453,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="9" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>12</v>
@@ -3518,7 +3473,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="9" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
@@ -3538,10 +3493,10 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="9" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
@@ -3558,10 +3513,10 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="9" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
@@ -3578,10 +3533,10 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="9" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>
@@ -3598,10 +3553,10 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="9" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
@@ -3610,7 +3565,7 @@
         <v>3.5</v>
       </c>
       <c r="G7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H7">
         <v>345</v>
@@ -3618,10 +3573,10 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="9" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
         <v>13</v>
@@ -3630,7 +3585,7 @@
         <v>3.5</v>
       </c>
       <c r="G8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H8">
         <v>345</v>
@@ -3638,10 +3593,10 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="9" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
         <v>13</v>
@@ -3650,7 +3605,7 @@
         <v>3.5</v>
       </c>
       <c r="G9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H9">
         <v>345</v>
@@ -3658,10 +3613,10 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="9" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
         <v>13</v>
@@ -3670,7 +3625,7 @@
         <v>3.5</v>
       </c>
       <c r="G10" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="H10">
         <v>360</v>
@@ -3678,10 +3633,10 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="9" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -3690,7 +3645,7 @@
         <v>3.5</v>
       </c>
       <c r="G11" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="H11">
         <v>351</v>
@@ -3698,10 +3653,10 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="9" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
         <v>13</v>
@@ -3710,7 +3665,7 @@
         <v>3.5</v>
       </c>
       <c r="G12" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="H12">
         <v>351</v>
@@ -3718,10 +3673,10 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="9" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s">
         <v>13</v>
@@ -3730,7 +3685,7 @@
         <v>3.5</v>
       </c>
       <c r="G13" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="H13">
         <v>351</v>
@@ -3738,10 +3693,10 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="9" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D14" t="s">
         <v>13</v>
@@ -3750,7 +3705,7 @@
         <v>4.7</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="H14">
         <v>510</v>
@@ -3758,10 +3713,10 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="9" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D15" t="s">
         <v>13</v>
@@ -3770,7 +3725,7 @@
         <v>4.7</v>
       </c>
       <c r="G15" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="H15">
         <v>510</v>
@@ -3778,10 +3733,10 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="9" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B16" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="D16" t="s">
         <v>13</v>
@@ -3790,7 +3745,7 @@
         <v>4.7</v>
       </c>
       <c r="G16" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="H16">
         <v>510</v>
@@ -3798,10 +3753,10 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="9" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="D17" t="s">
         <v>13</v>
@@ -3810,7 +3765,7 @@
         <v>4.7</v>
       </c>
       <c r="G17" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="H17">
         <v>510</v>
@@ -3851,57 +3806,57 @@
   <sheetData>
     <row r="1" ht="23.25" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="L1" s="7"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="E2" s="4">
         <v>2.6</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="4" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="H2" s="4">
         <v>235</v>
@@ -3913,21 +3868,21 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="2" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="E3" s="4">
         <v>2.6</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="4" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="H3" s="4">
         <v>235</v>
@@ -3939,21 +3894,21 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="2" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="E4" s="4">
         <v>2.6</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="4" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="H4" s="4">
         <v>240</v>
@@ -3965,21 +3920,21 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="2" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="E5" s="3">
         <v>2.8</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="4" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="H5" s="4">
         <v>356</v>
@@ -3991,21 +3946,21 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="2" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="E6" s="3">
         <v>2.8</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="4" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="H6" s="4">
         <v>356</v>
@@ -4017,19 +3972,19 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="2" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="E7" s="3">
         <v>2.8</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="H7" s="4">
         <v>356</v>
@@ -4040,19 +3995,19 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="2" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="E8" s="3">
         <v>2.8</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="H8" s="4">
         <v>356</v>
@@ -4063,19 +4018,19 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="2" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="E9" s="4">
         <v>2.8</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="H9" s="4">
         <v>389</v>
@@ -4086,19 +4041,19 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="2" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="E10" s="4">
         <v>2.8</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="H10" s="4">
         <v>389</v>
@@ -4109,19 +4064,19 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="2" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="E11" s="4">
         <v>2.8</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="H11" s="4">
         <v>389</v>
@@ -4132,19 +4087,19 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="2" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="E12" s="4">
         <v>2.8</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="H12" s="4">
         <v>388</v>
@@ -4155,19 +4110,19 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="2" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="E13" s="4">
         <v>2.8</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="H13" s="4">
         <v>388</v>
@@ -4178,10 +4133,10 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="2" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>13</v>
@@ -4190,7 +4145,7 @@
         <v>2.8</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="H14" s="4">
         <v>391</v>
@@ -4201,19 +4156,19 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="2" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="E15" s="4">
         <v>2.8</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="H15" s="4">
         <v>391</v>
@@ -4224,19 +4179,19 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="2" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="B16" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="E16" s="4">
         <v>2.8</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="H16" s="4">
         <v>391</v>
@@ -4247,19 +4202,19 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="2" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="B17" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="E17" s="4">
         <v>2.8</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="H17" s="4">
         <v>391</v>
@@ -4270,19 +4225,19 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="2" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="B18" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="E18" s="4">
         <v>2.8</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="H18" s="4">
         <v>391</v>
@@ -4293,19 +4248,19 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="2" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="B19" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="E19" s="4">
         <v>2.8</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="H19" s="4">
         <v>391</v>
@@ -4316,19 +4271,19 @@
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="2" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="E20" s="4">
         <v>4.2</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="H20" s="4">
         <v>429</v>
@@ -4339,19 +4294,19 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="2" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="B21" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="E21" s="4">
         <v>4.2</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="H21" s="4">
         <v>429</v>
@@ -4362,19 +4317,19 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="2" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="E22" s="4">
         <v>4.2</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="H22" s="4">
         <v>429</v>
@@ -4385,19 +4340,19 @@
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="2" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="E23" s="4">
         <v>4.2</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="H23" s="4">
         <v>429</v>
@@ -4408,19 +4363,19 @@
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="2" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="B24" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="E24">
         <v>3.7</v>
       </c>
       <c r="G24" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="H24">
         <v>374</v>
@@ -4431,19 +4386,19 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="2" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="B25" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="E25">
         <v>3.7</v>
       </c>
       <c r="G25" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="H25">
         <v>374</v>
@@ -4451,19 +4406,19 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="2" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="E26">
         <v>3.7</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="H26" s="4">
         <v>353</v>
@@ -4471,19 +4426,19 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="2" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="D27" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="E27">
         <v>3.7</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="H27" s="4">
         <v>358</v>
@@ -4491,19 +4446,19 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="2" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="D28" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="E28">
         <v>3.7</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="H28" s="4">
         <v>336</v>
@@ -4511,19 +4466,19 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="2" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="D29" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="E29" s="4">
         <v>3.7</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="H29" s="4">
         <v>336</v>
@@ -4531,19 +4486,19 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="2" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="D30" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="E30" s="4">
         <v>3.4</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="H30" s="4">
         <v>240</v>
@@ -4551,19 +4506,19 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="2" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="D31" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="E31" s="4">
         <v>3.7</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="H31" s="4">
         <v>333</v>
@@ -4571,19 +4526,19 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="2" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="D32" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="E32" s="4">
         <v>3.7</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="H32" s="4">
         <v>371</v>
@@ -4591,19 +4546,19 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="2" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="D33" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="E33" s="4">
         <v>3.7</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="H33">
         <v>371</v>
@@ -4611,19 +4566,19 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="2" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="D34" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="E34" s="4">
         <v>4.9</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="H34" s="4">
         <v>460</v>
@@ -4631,19 +4586,19 @@
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="2" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="D35" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="E35" s="4">
         <v>4.9</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="H35" s="4">
         <v>460</v>
@@ -4651,19 +4606,19 @@
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="2" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="D36" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="E36" s="4">
         <v>4.9</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="H36" s="4">
         <v>460</v>
@@ -4671,19 +4626,19 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="2" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="D37" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="E37" s="4">
         <v>5.6</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="H37" s="4">
         <v>563</v>
@@ -4691,19 +4646,19 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="2" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="D38" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="E38" s="4">
         <v>3.1</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="H38" s="4">
         <v>356</v>
@@ -4711,19 +4666,19 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="2" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="D39" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="E39" s="4">
         <v>3.1</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="H39" s="4">
         <v>379</v>
@@ -4731,19 +4686,19 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="2" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="D40" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="E40" s="4">
         <v>3.1</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="H40" s="4">
         <v>379</v>
@@ -4751,19 +4706,19 @@
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="2" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="D41" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="E41" s="4">
         <v>3.7</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="H41" s="4">
         <v>367</v>
@@ -4771,19 +4726,19 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="2" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="D42" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="E42" s="4">
         <v>3.7</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="H42" s="4">
         <v>363</v>
@@ -4791,19 +4746,19 @@
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="2" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="D43" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="E43" s="4">
         <v>3.4</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="H43" s="4">
         <v>246</v>
@@ -4811,19 +4766,19 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="2" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="D44" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="E44" s="4">
         <v>3.1</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="H44" s="4">
         <v>372</v>
@@ -4831,19 +4786,19 @@
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="2" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="D45" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="E45" s="4">
         <v>3.4</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="H45" s="4">
         <v>234</v>
@@ -4851,19 +4806,19 @@
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="2" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="D46" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="E46" s="4">
         <v>3.4</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="H46" s="4">
         <v>234</v>
@@ -4871,19 +4826,19 @@
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="2" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="D47" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="E47" s="4">
         <v>3.7</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="H47" s="4">
         <v>337</v>
@@ -4891,19 +4846,19 @@
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="2" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="D48" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="E48" s="4">
         <v>3.7</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="H48" s="4">
         <v>363</v>
@@ -4911,19 +4866,19 @@
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="2" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="D49" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="E49" s="4">
         <v>4.9</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="H49" s="4">
         <v>419</v>
@@ -4931,19 +4886,19 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="2" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="D50" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="E50" s="4">
         <v>3.1</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="H50" s="4">
         <v>358</v>
@@ -4951,19 +4906,19 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="2" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="D51" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="E51" s="4">
         <v>4.9</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="H51" s="4">
         <v>459</v>
@@ -4971,10 +4926,10 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="2" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="D52" t="s">
         <v>13</v>
@@ -4983,7 +4938,7 @@
         <v>2.8</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="H52" s="4">
         <v>398</v>
@@ -4991,19 +4946,19 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="2" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="D53" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="E53" s="4">
         <v>3.7</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="H53" s="4">
         <v>305</v>
@@ -5011,19 +4966,19 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="2" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="D54" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="E54" s="4">
         <v>3.7</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="H54" s="4">
         <v>335</v>
@@ -5031,19 +4986,19 @@
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="2" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="D55" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="E55" s="4">
         <v>3.7</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="H55" s="4">
         <v>379</v>
@@ -5051,19 +5006,19 @@
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="2" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="D56" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="E56" s="4">
         <v>4.2</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="H56" s="4">
         <v>353</v>
@@ -5071,19 +5026,19 @@
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="2" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="D57" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="E57" s="4">
         <v>3.7</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="H57" s="4">
         <v>334</v>
@@ -5091,19 +5046,19 @@
     </row>
     <row r="58" spans="1:8">
       <c r="A58" s="2" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="D58" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="E58" s="4">
         <v>3.7</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="H58" s="4">
         <v>303</v>
@@ -5111,19 +5066,19 @@
     </row>
     <row r="59" spans="1:8">
       <c r="A59" s="2" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="D59" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="E59" s="4">
         <v>3.7</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="H59" s="4">
         <v>303</v>
@@ -5131,19 +5086,19 @@
     </row>
     <row r="60" spans="1:8">
       <c r="A60" s="2" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="D60" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="E60" s="4">
         <v>4.2</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="H60" s="4">
         <v>369</v>
@@ -5151,19 +5106,19 @@
     </row>
     <row r="61" spans="1:8">
       <c r="A61" s="2" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="D61" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="E61" s="4">
         <v>4.2</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="H61" s="4">
         <v>369</v>
@@ -5171,19 +5126,19 @@
     </row>
     <row r="62" spans="1:8">
       <c r="A62" s="2" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="D62" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="E62" s="4">
         <v>3.1</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="H62" s="4">
         <v>200</v>
@@ -5191,19 +5146,19 @@
     </row>
     <row r="63" spans="1:8">
       <c r="A63" s="2" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="D63" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="E63" s="4">
         <v>3.7</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="H63" s="4">
         <v>310</v>

</xml_diff>

<commit_message>
generating second catagory products Snap Closure Full Package also done
</commit_message>
<xml_diff>
--- a/ChaoKaiQiProducts.xlsx
+++ b/ChaoKaiQiProducts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21945" windowHeight="9720"/>
+    <workbookView windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Snap rotate style" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="227">
   <si>
     <t>Cover Name</t>
   </si>
@@ -171,7 +171,25 @@
     <t>200 * 160 * 15</t>
   </si>
   <si>
+    <t>/ProductImages/snapClosureFullPackage/snapClosureFullPackage (1)</t>
+  </si>
+  <si>
+    <t>/ProductImages/snapClosureFullPackage/snapClosureFullPackage (1),/ProductImages/snapClosureFullPackage/snapClosureFullPackage (2),/ProductImages/snapClosureFullPackage/snapClosureFullPackage (3),/ProductImages/snapClosureFullPackage/snapClosureFullPackage (4),/ProductImages/snapClosureFullPackage/snapClosureFullPackage (5),/ProductImages/snapClosureFullPackage/colors/black,/ProductImages/snapClosureFullPackage/colors/whiteIce,/ProductImages/snapClosureFullPackage/colors/deepGreen,/ProductImages/snapClosureFullPackage/colors/babyPink,/ProductImages/snapClosureFullPackage/colors/gray,/ProductImages/snapClosureFullPackage/colors/lavanderPurple</t>
+  </si>
+  <si>
     <t>245 * 195 * 18</t>
+  </si>
+  <si>
+    <t>/ProductImages/snapClosureFullPackage/snapClosureFullPackage (2)</t>
+  </si>
+  <si>
+    <t>/ProductImages/snapClosureFullPackage/snapClosureFullPackage (3)</t>
+  </si>
+  <si>
+    <t>/ProductImages/snapClosureFullPackage/snapClosureFullPackage (4)</t>
+  </si>
+  <si>
+    <t>/ProductImages/snapClosureFullPackage/snapClosureFullPackage (5)</t>
   </si>
   <si>
     <t>253 * 190 * 18</t>
@@ -1950,7 +1968,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1976,9 +1994,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -2525,8 +2540,8 @@
   <sheetPr/>
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -2536,10 +2551,10 @@
     <col min="3" max="3" width="22.5714285714286" customWidth="1"/>
     <col min="4" max="4" width="17.8571428571429" customWidth="1"/>
     <col min="5" max="5" width="15.7142857142857" customWidth="1"/>
-    <col min="6" max="6" width="5" customWidth="1"/>
+    <col min="6" max="6" width="15.2857142857143" customWidth="1"/>
     <col min="7" max="7" width="13.8571428571429" customWidth="1"/>
-    <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="55" customWidth="1"/>
+    <col min="8" max="8" width="20.1428571428571" customWidth="1"/>
+    <col min="9" max="9" width="61.4285714285714" customWidth="1"/>
     <col min="10" max="10" width="60.7142857142857" customWidth="1"/>
     <col min="11" max="11" width="22.4285714285714" customWidth="1"/>
     <col min="12" max="13" width="20.8571428571429" customWidth="1"/>
@@ -2579,17 +2594,17 @@
       <c r="K1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D2" t="s">
@@ -2612,7 +2627,7 @@
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B3" t="s">
@@ -2638,7 +2653,7 @@
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B4" t="s">
@@ -2664,7 +2679,7 @@
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B5" t="s">
@@ -2690,7 +2705,7 @@
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B6" t="s">
@@ -2716,7 +2731,7 @@
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B7" t="s">
@@ -2742,7 +2757,7 @@
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B8" t="s">
@@ -2768,7 +2783,7 @@
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B9" t="s">
@@ -2794,7 +2809,7 @@
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B10" t="s">
@@ -2820,7 +2835,7 @@
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B11" t="s">
@@ -2846,7 +2861,7 @@
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B12" t="s">
@@ -2872,7 +2887,7 @@
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
@@ -2898,7 +2913,7 @@
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B14" t="s">
@@ -2924,7 +2939,7 @@
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B15" t="s">
@@ -2950,7 +2965,7 @@
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B16" t="s">
@@ -2976,7 +2991,7 @@
       </c>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B17" t="s">
@@ -3012,8 +3027,8 @@
   <sheetPr/>
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -3026,8 +3041,8 @@
     <col min="6" max="6" width="6.14285714285714" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="18.1428571428571" customWidth="1"/>
-    <col min="10" max="10" width="28.4285714285714" customWidth="1"/>
+    <col min="9" max="9" width="64.5714285714286" customWidth="1"/>
+    <col min="10" max="10" width="63" customWidth="1"/>
     <col min="11" max="11" width="22.4285714285714" customWidth="1"/>
     <col min="12" max="13" width="20.8571428571429" customWidth="1"/>
   </cols>
@@ -3066,17 +3081,17 @@
       <c r="K1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-    </row>
-    <row r="2" customFormat="1" spans="1:8">
-      <c r="A2" s="9" t="s">
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+    </row>
+    <row r="2" customFormat="1" spans="1:10">
+      <c r="A2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D2" t="s">
@@ -3091,9 +3106,15 @@
       <c r="H2">
         <v>259</v>
       </c>
-    </row>
-    <row r="3" customFormat="1" spans="1:8">
-      <c r="A3" s="9" t="s">
+      <c r="I2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" customFormat="1" spans="1:10">
+      <c r="A3" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B3" t="s">
@@ -3106,14 +3127,20 @@
         <v>3.5</v>
       </c>
       <c r="G3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H3">
         <v>368</v>
       </c>
-    </row>
-    <row r="4" customFormat="1" spans="1:8">
-      <c r="A4" s="9" t="s">
+      <c r="I3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" customFormat="1" spans="1:10">
+      <c r="A4" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B4" t="s">
@@ -3126,14 +3153,20 @@
         <v>3.5</v>
       </c>
       <c r="G4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H4">
         <v>368</v>
       </c>
-    </row>
-    <row r="5" customFormat="1" spans="1:8">
-      <c r="A5" s="9" t="s">
+      <c r="I4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" customFormat="1" spans="1:10">
+      <c r="A5" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B5" t="s">
@@ -3146,14 +3179,20 @@
         <v>3.5</v>
       </c>
       <c r="G5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H5">
         <v>368</v>
       </c>
-    </row>
-    <row r="6" customFormat="1" spans="1:8">
-      <c r="A6" s="9" t="s">
+      <c r="I5" t="s">
+        <v>52</v>
+      </c>
+      <c r="J5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" customFormat="1" spans="1:10">
+      <c r="A6" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B6" t="s">
@@ -3166,14 +3205,20 @@
         <v>3.5</v>
       </c>
       <c r="G6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H6">
         <v>368</v>
       </c>
-    </row>
-    <row r="7" customFormat="1" spans="1:8">
-      <c r="A7" s="9" t="s">
+      <c r="I6" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" customFormat="1" spans="1:10">
+      <c r="A7" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B7" t="s">
@@ -3186,14 +3231,20 @@
         <v>3.5</v>
       </c>
       <c r="G7" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="H7">
         <v>434</v>
       </c>
-    </row>
-    <row r="8" customFormat="1" spans="1:8">
-      <c r="A8" s="9" t="s">
+      <c r="I7" t="s">
+        <v>47</v>
+      </c>
+      <c r="J7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" customFormat="1" spans="1:10">
+      <c r="A8" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B8" t="s">
@@ -3206,14 +3257,20 @@
         <v>3.5</v>
       </c>
       <c r="G8" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="H8">
         <v>434</v>
       </c>
-    </row>
-    <row r="9" customFormat="1" spans="1:8">
-      <c r="A9" s="9" t="s">
+      <c r="I8" t="s">
+        <v>50</v>
+      </c>
+      <c r="J8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" customFormat="1" spans="1:10">
+      <c r="A9" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B9" t="s">
@@ -3226,14 +3283,20 @@
         <v>3.5</v>
       </c>
       <c r="G9" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="H9">
         <v>434</v>
       </c>
-    </row>
-    <row r="10" customFormat="1" spans="1:8">
-      <c r="A10" s="9" t="s">
+      <c r="I9" t="s">
+        <v>51</v>
+      </c>
+      <c r="J9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" customFormat="1" spans="1:10">
+      <c r="A10" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B10" t="s">
@@ -3246,14 +3309,20 @@
         <v>3.5</v>
       </c>
       <c r="G10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="H10">
         <v>357</v>
       </c>
-    </row>
-    <row r="11" customFormat="1" spans="1:8">
-      <c r="A11" s="9" t="s">
+      <c r="I10" t="s">
+        <v>52</v>
+      </c>
+      <c r="J10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" customFormat="1" spans="1:10">
+      <c r="A11" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B11" t="s">
@@ -3266,14 +3335,20 @@
         <v>3.5</v>
       </c>
       <c r="G11" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="H11">
         <v>432</v>
       </c>
-    </row>
-    <row r="12" customFormat="1" spans="1:8">
-      <c r="A12" s="9" t="s">
+      <c r="I11" t="s">
+        <v>53</v>
+      </c>
+      <c r="J11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" customFormat="1" spans="1:10">
+      <c r="A12" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B12" t="s">
@@ -3286,14 +3361,20 @@
         <v>3.5</v>
       </c>
       <c r="G12" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="H12">
         <v>432</v>
       </c>
-    </row>
-    <row r="13" customFormat="1" spans="1:8">
-      <c r="A13" s="9" t="s">
+      <c r="I12" t="s">
+        <v>47</v>
+      </c>
+      <c r="J12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" customFormat="1" spans="1:10">
+      <c r="A13" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B13" t="s">
@@ -3306,14 +3387,20 @@
         <v>3.5</v>
       </c>
       <c r="G13" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="H13">
         <v>432</v>
       </c>
-    </row>
-    <row r="14" customFormat="1" spans="1:8">
-      <c r="A14" s="9" t="s">
+      <c r="I13" t="s">
+        <v>50</v>
+      </c>
+      <c r="J13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" customFormat="1" spans="1:10">
+      <c r="A14" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B14" t="s">
@@ -3325,15 +3412,21 @@
       <c r="E14">
         <v>4.7</v>
       </c>
-      <c r="G14" s="10" t="s">
-        <v>51</v>
+      <c r="G14" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="H14">
         <v>551</v>
       </c>
-    </row>
-    <row r="15" customFormat="1" spans="1:8">
-      <c r="A15" s="9" t="s">
+      <c r="I14" t="s">
+        <v>51</v>
+      </c>
+      <c r="J14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" customFormat="1" spans="1:10">
+      <c r="A15" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B15" t="s">
@@ -3346,14 +3439,20 @@
         <v>4.7</v>
       </c>
       <c r="G15" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="H15">
         <v>551</v>
       </c>
-    </row>
-    <row r="16" customFormat="1" spans="1:8">
-      <c r="A16" s="9" t="s">
+      <c r="I15" t="s">
+        <v>52</v>
+      </c>
+      <c r="J15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" customFormat="1" spans="1:10">
+      <c r="A16" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B16" t="s">
@@ -3366,14 +3465,20 @@
         <v>4.7</v>
       </c>
       <c r="G16" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="H16">
         <v>551</v>
       </c>
-    </row>
-    <row r="17" customFormat="1" spans="1:8">
-      <c r="A17" s="9" t="s">
+      <c r="I16" t="s">
+        <v>53</v>
+      </c>
+      <c r="J16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" customFormat="1" spans="1:10">
+      <c r="A17" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B17" t="s">
@@ -3386,10 +3491,16 @@
         <v>4.7</v>
       </c>
       <c r="G17" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="H17">
         <v>551</v>
+      </c>
+      <c r="I17" t="s">
+        <v>47</v>
+      </c>
+      <c r="J17" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -3449,13 +3560,13 @@
       <c r="K1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="12"/>
+      <c r="L1" s="11"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B2" s="10" t="s">
+      <c r="A2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D2" t="s">
@@ -3472,8 +3583,8 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="9" t="s">
-        <v>52</v>
+      <c r="A3" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
@@ -3492,8 +3603,8 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="9" t="s">
-        <v>52</v>
+      <c r="A4" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
@@ -3512,8 +3623,8 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="9" t="s">
-        <v>52</v>
+      <c r="A5" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="B5" t="s">
         <v>23</v>
@@ -3532,8 +3643,8 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="9" t="s">
-        <v>52</v>
+      <c r="A6" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="B6" t="s">
         <v>25</v>
@@ -3552,8 +3663,8 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="9" t="s">
-        <v>52</v>
+      <c r="A7" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="B7" t="s">
         <v>27</v>
@@ -3572,8 +3683,8 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="9" t="s">
-        <v>52</v>
+      <c r="A8" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="B8" t="s">
         <v>30</v>
@@ -3592,8 +3703,8 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="9" t="s">
-        <v>52</v>
+      <c r="A9" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="B9" t="s">
         <v>32</v>
@@ -3612,8 +3723,8 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="9" t="s">
-        <v>52</v>
+      <c r="A10" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="B10" t="s">
         <v>34</v>
@@ -3625,15 +3736,15 @@
         <v>3.5</v>
       </c>
       <c r="G10" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="H10">
         <v>360</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="9" t="s">
-        <v>52</v>
+      <c r="A11" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="B11" t="s">
         <v>36</v>
@@ -3652,8 +3763,8 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="9" t="s">
-        <v>52</v>
+      <c r="A12" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="B12" t="s">
         <v>38</v>
@@ -3672,8 +3783,8 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="9" t="s">
-        <v>52</v>
+      <c r="A13" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="B13" t="s">
         <v>39</v>
@@ -3692,8 +3803,8 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="9" t="s">
-        <v>52</v>
+      <c r="A14" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="B14" t="s">
         <v>40</v>
@@ -3704,16 +3815,16 @@
       <c r="E14">
         <v>4.7</v>
       </c>
-      <c r="G14" s="10" t="s">
-        <v>54</v>
+      <c r="G14" s="9" t="s">
+        <v>60</v>
       </c>
       <c r="H14">
         <v>510</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="9" t="s">
-        <v>52</v>
+      <c r="A15" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="B15" t="s">
         <v>42</v>
@@ -3725,15 +3836,15 @@
         <v>4.7</v>
       </c>
       <c r="G15" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="H15">
         <v>510</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="9" t="s">
-        <v>52</v>
+      <c r="A16" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="B16" t="s">
         <v>43</v>
@@ -3745,15 +3856,15 @@
         <v>4.7</v>
       </c>
       <c r="G16" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="H16">
         <v>510</v>
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="9" t="s">
-        <v>52</v>
+      <c r="A17" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="B17" t="s">
         <v>44</v>
@@ -3765,15 +3876,15 @@
         <v>4.7</v>
       </c>
       <c r="G17" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="H17">
         <v>510</v>
       </c>
     </row>
     <row r="22" spans="2:4">
-      <c r="B22" s="9"/>
-      <c r="D22" s="11"/>
+      <c r="B22" s="4"/>
+      <c r="D22" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3786,7 +3897,7 @@
   <sheetPr/>
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
@@ -3806,57 +3917,57 @@
   <sheetData>
     <row r="1" ht="23.25" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="L1" s="7"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E2" s="4">
         <v>2.6</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="4" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="H2" s="4">
         <v>235</v>
@@ -3868,21 +3979,21 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E3" s="4">
         <v>2.6</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="4" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="H3" s="4">
         <v>235</v>
@@ -3894,21 +4005,21 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="2" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E4" s="4">
         <v>2.6</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="4" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="H4" s="4">
         <v>240</v>
@@ -3920,21 +4031,21 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="2" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E5" s="3">
         <v>2.8</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="4" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="H5" s="4">
         <v>356</v>
@@ -3946,21 +4057,21 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="2" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="B6" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E6" s="3">
         <v>2.8</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="4" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="H6" s="4">
         <v>356</v>
@@ -3972,19 +4083,19 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="2" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="B7" t="s">
         <v>23</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E7" s="3">
         <v>2.8</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="H7" s="4">
         <v>356</v>
@@ -3995,19 +4106,19 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="2" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="B8" t="s">
         <v>25</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E8" s="3">
         <v>2.8</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="H8" s="4">
         <v>356</v>
@@ -4018,19 +4129,19 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="2" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B9" t="s">
         <v>27</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E9" s="4">
         <v>2.8</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="H9" s="4">
         <v>389</v>
@@ -4041,19 +4152,19 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="2" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B10" t="s">
         <v>30</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E10" s="4">
         <v>2.8</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="H10" s="4">
         <v>389</v>
@@ -4064,19 +4175,19 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="2" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B11" t="s">
         <v>32</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E11" s="4">
         <v>2.8</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="H11" s="4">
         <v>389</v>
@@ -4087,19 +4198,19 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="2" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E12" s="4">
         <v>2.8</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="H12" s="4">
         <v>388</v>
@@ -4110,19 +4221,19 @@
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="2" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E13" s="4">
         <v>2.8</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="H13" s="4">
         <v>388</v>
@@ -4133,7 +4244,7 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="2" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B14" t="s">
         <v>38</v>
@@ -4145,7 +4256,7 @@
         <v>2.8</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="H14" s="4">
         <v>391</v>
@@ -4156,19 +4267,19 @@
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="2" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B15" t="s">
         <v>39</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E15" s="4">
         <v>2.8</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="H15" s="4">
         <v>391</v>
@@ -4179,19 +4290,19 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="2" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B16" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E16" s="4">
         <v>2.8</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="H16" s="4">
         <v>391</v>
@@ -4202,19 +4313,19 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="2" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B17" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E17" s="4">
         <v>2.8</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="H17" s="4">
         <v>391</v>
@@ -4225,19 +4336,19 @@
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="2" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B18" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E18" s="4">
         <v>2.8</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="H18" s="4">
         <v>391</v>
@@ -4248,19 +4359,19 @@
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="2" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B19" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E19" s="4">
         <v>2.8</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="H19" s="4">
         <v>391</v>
@@ -4271,19 +4382,19 @@
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="2" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B20" t="s">
         <v>40</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E20" s="4">
         <v>4.2</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="H20" s="4">
         <v>429</v>
@@ -4294,19 +4405,19 @@
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="2" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B21" t="s">
         <v>42</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E21" s="4">
         <v>4.2</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="H21" s="4">
         <v>429</v>
@@ -4317,19 +4428,19 @@
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="2" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B22" t="s">
         <v>43</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E22" s="4">
         <v>4.2</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="H22" s="4">
         <v>429</v>
@@ -4340,19 +4451,19 @@
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="2" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B23" t="s">
         <v>44</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E23" s="4">
         <v>4.2</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="H23" s="4">
         <v>429</v>
@@ -4363,19 +4474,19 @@
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="2" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B24" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="E24">
         <v>3.7</v>
       </c>
       <c r="G24" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="H24">
         <v>374</v>
@@ -4386,19 +4497,19 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="2" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B25" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="E25">
         <v>3.7</v>
       </c>
       <c r="G25" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="H25">
         <v>374</v>
@@ -4406,19 +4517,19 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="2" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="E26">
         <v>3.7</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="H26" s="4">
         <v>353</v>
@@ -4426,19 +4537,19 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="2" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="D27" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="E27">
         <v>3.7</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="H27" s="4">
         <v>358</v>
@@ -4446,19 +4557,19 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="2" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="D28" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="E28">
         <v>3.7</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="H28" s="4">
         <v>336</v>
@@ -4466,19 +4577,19 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="2" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="B29" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D29" t="s">
         <v>121</v>
-      </c>
-      <c r="D29" t="s">
-        <v>115</v>
       </c>
       <c r="E29" s="4">
         <v>3.7</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="H29" s="4">
         <v>336</v>
@@ -4486,19 +4597,19 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="2" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="D30" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="E30" s="4">
         <v>3.4</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="H30" s="4">
         <v>240</v>
@@ -4506,19 +4617,19 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="2" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="D31" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="E31" s="4">
         <v>3.7</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="H31" s="4">
         <v>333</v>
@@ -4526,19 +4637,19 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="2" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="D32" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="E32" s="4">
         <v>3.7</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="H32" s="4">
         <v>371</v>
@@ -4546,19 +4657,19 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="2" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="D33" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="E33" s="4">
         <v>3.7</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="H33">
         <v>371</v>
@@ -4566,19 +4677,19 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="2" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="D34" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="E34" s="4">
         <v>4.9</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="H34" s="4">
         <v>460</v>
@@ -4586,19 +4697,19 @@
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="2" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="D35" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="E35" s="4">
         <v>4.9</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="H35" s="4">
         <v>460</v>
@@ -4606,19 +4717,19 @@
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="2" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="D36" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="E36" s="4">
         <v>4.9</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="H36" s="4">
         <v>460</v>
@@ -4626,19 +4737,19 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="2" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="D37" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="E37" s="4">
         <v>5.6</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="H37" s="4">
         <v>563</v>
@@ -4646,19 +4757,19 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="2" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="D38" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="E38" s="4">
         <v>3.1</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="H38" s="4">
         <v>356</v>
@@ -4666,19 +4777,19 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="2" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="D39" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="E39" s="4">
         <v>3.1</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="H39" s="4">
         <v>379</v>
@@ -4686,19 +4797,19 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="2" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="B40" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D40" t="s">
         <v>151</v>
-      </c>
-      <c r="D40" t="s">
-        <v>145</v>
       </c>
       <c r="E40" s="4">
         <v>3.1</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="H40" s="4">
         <v>379</v>
@@ -4706,19 +4817,19 @@
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="2" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="D41" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="E41" s="4">
         <v>3.7</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="H41" s="4">
         <v>367</v>
@@ -4726,19 +4837,19 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="2" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="D42" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="E42" s="4">
         <v>3.7</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="H42" s="4">
         <v>363</v>
@@ -4746,19 +4857,19 @@
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="2" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="D43" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="E43" s="4">
         <v>3.4</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="H43" s="4">
         <v>246</v>
@@ -4766,19 +4877,19 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="2" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="D44" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="E44" s="4">
         <v>3.1</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="H44" s="4">
         <v>372</v>
@@ -4786,19 +4897,19 @@
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="2" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="D45" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="E45" s="4">
         <v>3.4</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="H45" s="4">
         <v>234</v>
@@ -4806,19 +4917,19 @@
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="2" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="D46" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="E46" s="4">
         <v>3.4</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="H46" s="4">
         <v>234</v>
@@ -4826,19 +4937,19 @@
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="2" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="D47" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="E47" s="4">
         <v>3.7</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="H47" s="4">
         <v>337</v>
@@ -4846,19 +4957,19 @@
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="2" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="D48" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="E48" s="4">
         <v>3.7</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="H48" s="4">
         <v>363</v>
@@ -4866,19 +4977,19 @@
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="2" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="D49" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="E49" s="4">
         <v>4.9</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="H49" s="4">
         <v>419</v>
@@ -4886,19 +4997,19 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="2" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="D50" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="E50" s="4">
         <v>3.1</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="H50" s="4">
         <v>358</v>
@@ -4906,19 +5017,19 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="2" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="D51" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="E51" s="4">
         <v>4.9</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="H51" s="4">
         <v>459</v>
@@ -4926,10 +5037,10 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="2" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="D52" t="s">
         <v>13</v>
@@ -4938,7 +5049,7 @@
         <v>2.8</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="H52" s="4">
         <v>398</v>
@@ -4946,19 +5057,19 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="2" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="D53" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="E53" s="4">
         <v>3.7</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="H53" s="4">
         <v>305</v>
@@ -4966,19 +5077,19 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="2" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="D54" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="E54" s="4">
         <v>3.7</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="H54" s="4">
         <v>335</v>
@@ -4986,19 +5097,19 @@
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="2" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="D55" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="E55" s="4">
         <v>3.7</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="H55" s="4">
         <v>379</v>
@@ -5006,19 +5117,19 @@
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="2" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="D56" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="E56" s="4">
         <v>4.2</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="H56" s="4">
         <v>353</v>
@@ -5026,19 +5137,19 @@
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="2" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="D57" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="E57" s="4">
         <v>3.7</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="H57" s="4">
         <v>334</v>
@@ -5046,19 +5157,19 @@
     </row>
     <row r="58" spans="1:8">
       <c r="A58" s="2" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="D58" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="E58" s="4">
         <v>3.7</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="H58" s="4">
         <v>303</v>
@@ -5066,19 +5177,19 @@
     </row>
     <row r="59" spans="1:8">
       <c r="A59" s="2" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="D59" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="E59" s="4">
         <v>3.7</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="H59" s="4">
         <v>303</v>
@@ -5086,19 +5197,19 @@
     </row>
     <row r="60" spans="1:8">
       <c r="A60" s="2" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="D60" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="E60" s="4">
         <v>4.2</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="H60" s="4">
         <v>369</v>
@@ -5106,19 +5217,19 @@
     </row>
     <row r="61" spans="1:8">
       <c r="A61" s="2" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="D61" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="E61" s="4">
         <v>4.2</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
       <c r="H61" s="4">
         <v>369</v>
@@ -5126,19 +5237,19 @@
     </row>
     <row r="62" spans="1:8">
       <c r="A62" s="2" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="D62" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="E62" s="4">
         <v>3.1</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="H62" s="4">
         <v>200</v>
@@ -5146,19 +5257,19 @@
     </row>
     <row r="63" spans="1:8">
       <c r="A63" s="2" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="D63" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="E63" s="4">
         <v>3.7</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="H63" s="4">
         <v>310</v>

</xml_diff>

<commit_message>
acrylic 360 degree rotating protective case, added, delete api made to delete any product starts with a specific name
</commit_message>
<xml_diff>
--- a/ChaoKaiQiProducts.xlsx
+++ b/ChaoKaiQiProducts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12210"/>
+    <workbookView windowWidth="28800" windowHeight="12210" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Snap rotate style" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="210">
   <si>
     <t>Cover Name</t>
   </si>
@@ -353,6 +353,23 @@
   <si>
     <r>
       <rPr>
+        <sz val="11.05"/>
+        <color rgb="FF000000"/>
+        <rFont val="CIDFont"/>
+        <charset val="134"/>
+      </rPr>
+      <t>210*150*13.5</t>
+    </r>
+  </si>
+  <si>
+    <t>/ProductImages/Acrylic360DegreeRotatingP/apple (1)</t>
+  </si>
+  <si>
+    <t>/ProductImages/Acrylic360DegreeRotatingP/apple (1),/ProductImages/Acrylic360DegreeRotatingP/apple (2),/ProductImages/Acrylic360DegreeRotatingP/apple (3),/ProductImages/Acrylic360DegreeRotatingP/apple (4),/ProductImages/Acrylic360DegreeRotatingP/colors/apple (1),/ProductImages/Acrylic360DegreeRotatingP/colors/apple (2),/ProductImages/Acrylic360DegreeRotatingP/colors/apple (3),/ProductImages/Acrylic360DegreeRotatingP/colors/apple (4),/ProductImages/Acrylic360DegreeRotatingP/colors/apple (5),/ProductImages/Acrylic360DegreeRotatingP/colors/apple (6)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
@@ -362,6 +379,9 @@
     </r>
   </si>
   <si>
+    <t>/ProductImages/Acrylic360DegreeRotatingP/apple (2)</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11.05"/>
@@ -369,11 +389,8 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>210*150*13.5</t>
-    </r>
-  </si>
-  <si>
-    <t>Acrylic 361-Degree Rotating Protective Case</t>
+      <t>iPad Mini6 8.3</t>
+    </r>
   </si>
   <si>
     <r>
@@ -383,8 +400,11 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>iPad Mini6 8.3</t>
-    </r>
+      <t>200*150*14.5</t>
+    </r>
+  </si>
+  <si>
+    <t>/ProductImages/Acrylic360DegreeRotatingP/apple (3)</t>
   </si>
   <si>
     <r>
@@ -394,11 +414,17 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>200*150*14.5</t>
-    </r>
-  </si>
-  <si>
-    <t>Acrylic 362-Degree Rotating Protective Case</t>
+      <t>245*184*15.3</t>
+    </r>
+  </si>
+  <si>
+    <t>/ProductImages/Acrylic360DegreeRotatingP/apple (4)</t>
+  </si>
+  <si>
+    <t>/ProductImages/Acrylic360DegreeRotatingP/colors/apple (1)</t>
+  </si>
+  <si>
+    <t>/ProductImages/Acrylic360DegreeRotatingP/colors/apple (2)</t>
   </si>
   <si>
     <r>
@@ -408,20 +434,20 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>245*184*15.3</t>
-    </r>
-  </si>
-  <si>
-    <t>Acrylic 363-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <t>Acrylic 364-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <t>Acrylic 365-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <t>Acrylic 366-Degree Rotating Protective Case</t>
+      <t>260*190*15.0</t>
+    </r>
+  </si>
+  <si>
+    <t>/ProductImages/Acrylic360DegreeRotatingP/colors/apple (3)</t>
+  </si>
+  <si>
+    <t>/ProductImages/Acrylic360DegreeRotatingP/colors/apple (4)</t>
+  </si>
+  <si>
+    <t>/ProductImages/Acrylic360DegreeRotatingP/colors/apple (5)</t>
+  </si>
+  <si>
+    <t>iPad Pro10.5</t>
   </si>
   <si>
     <r>
@@ -431,20 +457,14 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>260*190*15.0</t>
-    </r>
-  </si>
-  <si>
-    <t>Acrylic 367-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <t>Acrylic 368-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <t>Acrylic 369-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <t>iPad Pro10.5</t>
+      <t>255*190*13.2</t>
+    </r>
+  </si>
+  <si>
+    <t>/ProductImages/Acrylic360DegreeRotatingP/colors/apple (6)</t>
+  </si>
+  <si>
+    <t>iPad Air3</t>
   </si>
   <si>
     <r>
@@ -454,17 +474,20 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>255*190*13.2</t>
-    </r>
-  </si>
-  <si>
-    <t>Acrylic 370-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <t>iPad Air3</t>
-  </si>
-  <si>
-    <t>Acrylic 371-Degree Rotating Protective Case</t>
+      <t>251*190*14.5</t>
+    </r>
+  </si>
+  <si>
+    <t>ipad Pro 11 2018</t>
+  </si>
+  <si>
+    <t>ipad Pro 11 2020</t>
+  </si>
+  <si>
+    <t>ipad Pro 11 2021</t>
+  </si>
+  <si>
+    <t>ipad Pro 11 2022</t>
   </si>
   <si>
     <r>
@@ -474,38 +497,11 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>251*190*14.5</t>
-    </r>
-  </si>
-  <si>
-    <t>Acrylic 372-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <t>Acrylic 373-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <t>ipad Pro 11 2018</t>
-  </si>
-  <si>
-    <t>Acrylic 374-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <t>ipad Pro 11 2020</t>
-  </si>
-  <si>
-    <t>Acrylic 375-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <t>ipad Pro 11 2021</t>
-  </si>
-  <si>
-    <t>Acrylic 376-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <t>ipad Pro 11 2022</t>
-  </si>
-  <si>
-    <t>Acrylic 377-Degree Rotating Protective Case</t>
+      <t>286*230*16.0</t>
+    </r>
+  </si>
+  <si>
+    <t>iPad10 10.9 2022</t>
   </si>
   <si>
     <r>
@@ -515,38 +511,14 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>286*230*16.0</t>
-    </r>
-  </si>
-  <si>
-    <t>Acrylic 378-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <t>Acrylic 379-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <t>Acrylic 380-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <t>Acrylic 381-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <t>Mi 5</t>
-  </si>
-  <si>
-    <t>Xiaomi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">260*180*14.7 </t>
-  </si>
-  <si>
-    <t>Acrylic 382-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mi 5pro </t>
-  </si>
-  <si>
-    <t>Acrylic 383-Degree Rotating Protective Case</t>
+      <t>253*193*13.5</t>
+    </r>
+  </si>
+  <si>
+    <t>HONOR V7pro</t>
+  </si>
+  <si>
+    <t>HONOR</t>
   </si>
   <si>
     <r>
@@ -556,11 +528,14 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>Nokia T20</t>
-    </r>
-  </si>
-  <si>
-    <t>Nokia</t>
+      <t>260*180*19.5</t>
+    </r>
+  </si>
+  <si>
+    <t>/ProductImages/Acrylic360DegreeRotatingP/huawei (1)</t>
+  </si>
+  <si>
+    <t>HONOR 8 12" 2022</t>
   </si>
   <si>
     <r>
@@ -570,11 +545,17 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>253*173*14.7</t>
-    </r>
-  </si>
-  <si>
-    <t>Acrylic 384-Degree Rotating Protective Case</t>
+      <t>282*176*14.4</t>
+    </r>
+  </si>
+  <si>
+    <t>/ProductImages/Acrylic360DegreeRotatingP/huawei (2)</t>
+  </si>
+  <si>
+    <t>Huawei Matepad 10.4</t>
+  </si>
+  <si>
+    <t>Huawei</t>
   </si>
   <si>
     <r>
@@ -584,11 +565,14 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>TAB A8 10.5 2021</t>
-    </r>
-  </si>
-  <si>
-    <t>Samsung</t>
+      <t>250*171*20.5</t>
+    </r>
+  </si>
+  <si>
+    <t>/ProductImages/Acrylic360DegreeRotatingP/huawei (3)</t>
+  </si>
+  <si>
+    <t>Huawei Matepad 11</t>
   </si>
   <si>
     <r>
@@ -598,14 +582,20 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>253*180*14.4</t>
-    </r>
-  </si>
-  <si>
-    <t>Acrylic 385-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <t>TAB S6 Lite 10.4</t>
+      <t>260*180*15.3</t>
+    </r>
+  </si>
+  <si>
+    <t>/ProductImages/Acrylic360DegreeRotatingP/huawei (4)</t>
+  </si>
+  <si>
+    <t>Huawei Matepad 10.95</t>
+  </si>
+  <si>
+    <t>/ProductImages/Acrylic360DegreeRotatingP/huawei (5)</t>
+  </si>
+  <si>
+    <t>Huawei Matepad paper 10.3</t>
   </si>
   <si>
     <r>
@@ -615,25 +605,14 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>250*168*13.7</t>
-    </r>
-  </si>
-  <si>
-    <t>Acrylic 386-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11.05"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="CIDFont"/>
-        <charset val="134"/>
-      </rPr>
-      <t>TAB S6 Lite 2022</t>
-    </r>
-  </si>
-  <si>
-    <t>Acrylic 387-Degree Rotating Protective Case</t>
+      <t>233*200*13.5</t>
+    </r>
+  </si>
+  <si>
+    <t>/ProductImages/Acrylic360DegreeRotatingP/colors/huawei (1)</t>
+  </si>
+  <si>
+    <t>Huawei Matepad pro 11 2022</t>
   </si>
   <si>
     <r>
@@ -643,8 +622,11 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>TAB A7 Lite 8.7</t>
-    </r>
+      <t>253*172*13.5</t>
+    </r>
+  </si>
+  <si>
+    <t>/ProductImages/Acrylic360DegreeRotatingP/colors/huawei (2)</t>
   </si>
   <si>
     <r>
@@ -654,11 +636,11 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>218*140*14.5</t>
-    </r>
-  </si>
-  <si>
-    <t>Acrylic 388-Degree Rotating Protective Case</t>
+      <t>Huawei Matepad 11 2023</t>
+    </r>
+  </si>
+  <si>
+    <t>/ProductImages/Acrylic360DegreeRotatingP/colors/huawei (3)</t>
   </si>
   <si>
     <r>
@@ -668,7 +650,7 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>TAB A7 10.4 2020</t>
+      <t>Huawei Matepad Air 11.5 2023</t>
     </r>
   </si>
   <si>
@@ -679,14 +661,17 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>252*175*13.0</t>
-    </r>
-  </si>
-  <si>
-    <t>Acrylic 389-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <t>TAB S7 11</t>
+      <t>265*194*13.0</t>
+    </r>
+  </si>
+  <si>
+    <t>/ProductImages/Acrylic360DegreeRotatingP/colors/huawei (4)</t>
+  </si>
+  <si>
+    <t>Lenovo Y700 8.8</t>
+  </si>
+  <si>
+    <t>Lenovo</t>
   </si>
   <si>
     <r>
@@ -696,20 +681,20 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>260*182*18.5</t>
-    </r>
-  </si>
-  <si>
-    <t>Acrylic 390-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <t>TAB S8 11</t>
-  </si>
-  <si>
-    <t>Acrylic 391-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <t>TAB S7+ 12.4</t>
+      <t>210*144*15.6</t>
+    </r>
+  </si>
+  <si>
+    <t>/ProductImages/Acrylic360DegreeRotatingP/oppo (3)</t>
+  </si>
+  <si>
+    <t>/ProductImages/Acrylic360DegreeRotatingP/oppo (1),/ProductImages/Acrylic360DegreeRotatingP/oppo (2),/ProductImages/Acrylic360DegreeRotatingP/oppo (3),/ProductImages/Acrylic360DegreeRotatingP/oppo (4),/ProductImages/Acrylic360DegreeRotatingP/oppo (5),/ProductImages/Acrylic360DegreeRotatingP/colors/oppo (1),/ProductImages/Acrylic360DegreeRotatingP/colors/oppo (2),/ProductImages/Acrylic360DegreeRotatingP/colors/oppo (3),/ProductImages/Acrylic360DegreeRotatingP/colors/oppo (4),/ProductImages/Acrylic360DegreeRotatingP/colors/oppo (5),/ProductImages/Acrylic360DegreeRotatingP/colors/oppo (6)</t>
+  </si>
+  <si>
+    <t>Nokia T20</t>
+  </si>
+  <si>
+    <t>Nokia</t>
   </si>
   <si>
     <r>
@@ -719,23 +704,25 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>290*200*14.5</t>
-    </r>
-  </si>
-  <si>
-    <t>Acrylic 392-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <t>TAB S7 FE 12.4</t>
-  </si>
-  <si>
-    <t>Acrylic 393-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <t>TAB S8+ 12.4</t>
-  </si>
-  <si>
-    <t>Acrylic 394-Degree Rotating Protective Case</t>
+      <t>253*173*14.7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>/ProductImages/Acrylic360DegreeRotatingP/oppo (1),/ProductImages/Acrylic360DegreeRotatingP/oppo (2),/ProductImages/Acrylic360DegreeRotatingP/oppo (3),/ProductImages/Acrylic360DegreeRotatingP/oppo (4),/ProductImages/Acrylic360DegreeRotatingP/oppo (5),/ProductImages/Acrylic360DegreeRotatingP/colors/oppo (1),/ProductImages/Acrylic360DegreeRotatingP/colors/oppo (2),/ProductImages/Acrylic360DegreeRotatingP/colors/oppo (3),/ProductImages/Acrylic360DegreeRotatingP/colors/oppo (4),/ProductImages/Acrylic360DegreeRotatingP/colors/oppo (5),/ProductImages/Acrylic360DegreeRotatingP/colors/oppo (6)</t>
+    </r>
+  </si>
+  <si>
+    <t>OPPO pad 11 2022</t>
+  </si>
+  <si>
+    <t>OPPO</t>
   </si>
   <si>
     <r>
@@ -745,8 +732,14 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>TAB S8Ultra 14.6</t>
-    </r>
+      <t>260*180*15.0</t>
+    </r>
+  </si>
+  <si>
+    <t>/ProductImages/Acrylic360DegreeRotatingP/oppo (1)</t>
+  </si>
+  <si>
+    <t>OPPO Realme pad mini 8.7</t>
   </si>
   <si>
     <r>
@@ -756,17 +749,14 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>330*223*14.3</t>
-    </r>
-  </si>
-  <si>
-    <t>Acrylic 395-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <t>Huawei Matepad 10.4</t>
-  </si>
-  <si>
-    <t>Huawei</t>
+      <t>216*140*15.0</t>
+    </r>
+  </si>
+  <si>
+    <t>/ProductImages/Acrylic360DegreeRotatingP/oppo (2)</t>
+  </si>
+  <si>
+    <t>OPPO pad Air 10.3 2022</t>
   </si>
   <si>
     <r>
@@ -776,14 +766,11 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>250*171*20.5</t>
-    </r>
-  </si>
-  <si>
-    <t>Acrylic 396-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <t>Huawei Matepad 11</t>
+      <t>250*168*14.8</t>
+    </r>
+  </si>
+  <si>
+    <t>OPPO pad 2/11.6" 2023</t>
   </si>
   <si>
     <r>
@@ -793,23 +780,17 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>260*180*15.3</t>
-    </r>
-  </si>
-  <si>
-    <t>Acrylic 397-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <t>Huawei Matepad 10.95</t>
-  </si>
-  <si>
-    <t>Acrylic 398-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <t>HONOR V7pro</t>
-  </si>
-  <si>
-    <t>HONOR</t>
+      <t>263*203*13.0</t>
+    </r>
+  </si>
+  <si>
+    <t>/ProductImages/Acrylic360DegreeRotatingP/oppo (4)</t>
+  </si>
+  <si>
+    <t>TAB A8 10.5 2021</t>
+  </si>
+  <si>
+    <t>Samsung</t>
   </si>
   <si>
     <r>
@@ -819,17 +800,17 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>260*180*19.5</t>
-    </r>
-  </si>
-  <si>
-    <t>Acrylic 399-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <t>OPPO pad 11 2022</t>
-  </si>
-  <si>
-    <t>OPPO</t>
+      <t>253*180*14.4</t>
+    </r>
+  </si>
+  <si>
+    <t>/ProductImages/Acrylic360DegreeRotatingP/samsung (1)</t>
+  </si>
+  <si>
+    <t>/ProductImages/Acrylic360DegreeRotatingP/samsung (1),/ProductImages/Acrylic360DegreeRotatingP/samsung (2),/ProductImages/Acrylic360DegreeRotatingP/samsung (3),/ProductImages/Acrylic360DegreeRotatingP/samsung (4),/ProductImages/Acrylic360DegreeRotatingP/colors/samsung (1),/ProductImages/Acrylic360DegreeRotatingP/colors/samsung (2),/ProductImages/Acrylic360DegreeRotatingP/colors/samsung (3),/ProductImages/Acrylic360DegreeRotatingP/colors/samsung (4),/ProductImages/Acrylic360DegreeRotatingP/colors/samsung (5),/ProductImages/Acrylic360DegreeRotatingP/colors/samsung (6)</t>
+  </si>
+  <si>
+    <t>TAB S6 Lite 10.4</t>
   </si>
   <si>
     <r>
@@ -839,17 +820,20 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>260*180*15.0</t>
-    </r>
-  </si>
-  <si>
-    <t>Acrylic 400-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <t>Lenovo Y700 8.8</t>
-  </si>
-  <si>
-    <t>Lenovo</t>
+      <t>250*168*13.7</t>
+    </r>
+  </si>
+  <si>
+    <t>/ProductImages/Acrylic360DegreeRotatingP/samsung (2)</t>
+  </si>
+  <si>
+    <t>TAB S6 Lite 2022</t>
+  </si>
+  <si>
+    <t>/ProductImages/Acrylic360DegreeRotatingP/samsung (3)</t>
+  </si>
+  <si>
+    <t>TAB A7 Lite 8.7</t>
   </si>
   <si>
     <r>
@@ -859,14 +843,14 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>210*144*15.6</t>
-    </r>
-  </si>
-  <si>
-    <t>Acrylic 401-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <t>Huawei Matepad paper 10.3</t>
+      <t>218*140*14.5</t>
+    </r>
+  </si>
+  <si>
+    <t>/ProductImages/Acrylic360DegreeRotatingP/samsung (4)</t>
+  </si>
+  <si>
+    <t>TAB A7 10.4 2020</t>
   </si>
   <si>
     <r>
@@ -876,11 +860,14 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>233*200*13.5</t>
-    </r>
-  </si>
-  <si>
-    <t>Acrylic 402-Degree Rotating Protective Case</t>
+      <t>252*175*13.0</t>
+    </r>
+  </si>
+  <si>
+    <t>/ProductImages/Acrylic360DegreeRotatingP/colors/samsung (1)</t>
+  </si>
+  <si>
+    <t>TAB S7 11</t>
   </si>
   <si>
     <r>
@@ -890,8 +877,20 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>OPPO Realme pad mini 8.7</t>
-    </r>
+      <t>260*182*18.5</t>
+    </r>
+  </si>
+  <si>
+    <t>/ProductImages/Acrylic360DegreeRotatingP/colors/samsung (2)</t>
+  </si>
+  <si>
+    <t>TAB S8 11</t>
+  </si>
+  <si>
+    <t>/ProductImages/Acrylic360DegreeRotatingP/colors/samsung (3)</t>
+  </si>
+  <si>
+    <t>TAB S7+ 12.4</t>
   </si>
   <si>
     <r>
@@ -901,11 +900,26 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>216*140*15.0</t>
-    </r>
-  </si>
-  <si>
-    <t>Acrylic 403-Degree Rotating Protective Case</t>
+      <t>290*200*14.5</t>
+    </r>
+  </si>
+  <si>
+    <t>/ProductImages/Acrylic360DegreeRotatingP/colors/samsung (4)</t>
+  </si>
+  <si>
+    <t>TAB S7 FE 12.4</t>
+  </si>
+  <si>
+    <t>/ProductImages/Acrylic360DegreeRotatingP/colors/samsung (5)</t>
+  </si>
+  <si>
+    <t>TAB S8+ 12.4</t>
+  </si>
+  <si>
+    <t>/ProductImages/Acrylic360DegreeRotatingP/colors/samsung (6)</t>
+  </si>
+  <si>
+    <t>TAB S8Ultra 14.6</t>
   </si>
   <si>
     <r>
@@ -915,7 +929,7 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>TAB A8</t>
+      <t>330*223*14.3</t>
     </r>
   </si>
   <si>
@@ -926,11 +940,8 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>214*140*15.2</t>
-    </r>
-  </si>
-  <si>
-    <t>Acrylic 404-Degree Rotating Protective Case</t>
+      <t>TAB A8</t>
+    </r>
   </si>
   <si>
     <r>
@@ -940,7 +951,7 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>OPPO pad Air 10.3 2022</t>
+      <t>214*140*15.2</t>
     </r>
   </si>
   <si>
@@ -951,11 +962,8 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>250*168*14.8</t>
-    </r>
-  </si>
-  <si>
-    <t>Acrylic 405-Degree Rotating Protective Case</t>
+      <t>TAB S9 11 2023</t>
+    </r>
   </si>
   <si>
     <r>
@@ -965,17 +973,8 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>Vivo pad 11 2022</t>
-    </r>
-  </si>
-  <si>
-    <t>Vivo</t>
-  </si>
-  <si>
-    <t>Acrylic 406-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <t>HONOR 8 12" 2022</t>
+      <t>260*183*13.0</t>
+    </r>
   </si>
   <si>
     <r>
@@ -985,11 +984,8 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>282*176*14.4</t>
-    </r>
-  </si>
-  <si>
-    <t>Acrylic 407-Degree Rotating Protective Case</t>
+      <t>TAB S9FE 11 2023</t>
+    </r>
   </si>
   <si>
     <r>
@@ -999,7 +995,7 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>Huawei Matepad pro 11 2022</t>
+      <t>TAB S9+ 12.4 2023</t>
     </r>
   </si>
   <si>
@@ -1010,14 +1006,8 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>253*172*13.5</t>
-    </r>
-  </si>
-  <si>
-    <t>Acrylic 408-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <t>Xiaomi 5pro 12.4 2022</t>
+      <t>290*200*14.0</t>
+    </r>
   </si>
   <si>
     <r>
@@ -1027,11 +1017,8 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>209*200*15.0</t>
-    </r>
-  </si>
-  <si>
-    <t>Acrylic 409-Degree Rotating Protective Case</t>
+      <t>TAB S9+FE 12.4 2023</t>
+    </r>
   </si>
   <si>
     <r>
@@ -1041,7 +1028,7 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>iPad10 10.9 2022</t>
+      <t>TAB A9 8.7 2023</t>
     </r>
   </si>
   <si>
@@ -1052,11 +1039,8 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>253*193*13.5</t>
-    </r>
-  </si>
-  <si>
-    <t>Acrylic 410-Degree Rotating Protective Case</t>
+      <t>215*140*11.0</t>
+    </r>
   </si>
   <si>
     <r>
@@ -1066,7 +1050,7 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>Mi 6 2023</t>
+      <t>TAB A9+ 11 2023</t>
     </r>
   </si>
   <si>
@@ -1077,14 +1061,8 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>260*181*13.7</t>
-    </r>
-  </si>
-  <si>
-    <t>Acrylic 411-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <t>OPPO pad 2/11.6" 2023</t>
+      <t>260*185*14.0</t>
+    </r>
   </si>
   <si>
     <r>
@@ -1094,11 +1072,14 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>263*203*13.0</t>
-    </r>
-  </si>
-  <si>
-    <t>Acrylic 412-Degree Rotating Protective Case</t>
+      <t>Vivo pad 11 2022</t>
+    </r>
+  </si>
+  <si>
+    <t>Vivo</t>
+  </si>
+  <si>
+    <t>Vivo pad 2 12 2023</t>
   </si>
   <si>
     <r>
@@ -1108,14 +1089,59 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>Huawei Matepad 11 2023</t>
-    </r>
-  </si>
-  <si>
-    <t>Acrylic 413-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <t>Vivo pad 2 12 2023</t>
+      <t>273*210*14.0</t>
+    </r>
+  </si>
+  <si>
+    <t>Mi 5</t>
+  </si>
+  <si>
+    <t>Xiaomi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">260*180*14.7 </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF1E4D78"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>/ProductImages/Acrylic360DegreeRotatingP/xiaomi (2)</t>
+    </r>
+  </si>
+  <si>
+    <t>/ProductImages/Acrylic360DegreeRotatingP/xiaomi (5),/ProductImages/Acrylic360DegreeRotatingP/xiaomi (2),/ProductImages/Acrylic360DegreeRotatingP/xiaomi (3),/ProductImages/Acrylic360DegreeRotatingP/xiaomi (4),/ProductImages/Acrylic360DegreeRotatingP/colors/xiaomi (1),/ProductImages/Acrylic360DegreeRotatingP/colors/xiaomi (2),/ProductImages/Acrylic360DegreeRotatingP/colors/xiaomi (3),/ProductImages/Acrylic360DegreeRotatingP/colors/xiaomi (4),/ProductImages/Acrylic360DegreeRotatingP/colors/xiaomi (5),/ProductImages/Acrylic360DegreeRotatingP/colors/xiaomi (6)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mi 5pro </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF1E4D78"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>/ProductImages/Acrylic360DegreeRotatingP/xiaomi (3)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF1E4D78"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>/ProductImages/Acrylic360DegreeRotatingP/xiaomi (5),/ProductImages/Acrylic360DegreeRotatingP/xiaomi (2),/ProductImages/Acrylic360DegreeRotatingP/xiaomi (3),/ProductImages/Acrylic360DegreeRotatingP/xiaomi (4),/ProductImages/Acrylic360DegreeRotatingP/colors/xiaomi (1),/ProductImages/Acrylic360DegreeRotatingP/colors/xiaomi (2),/ProductImages/Acrylic360DegreeRotatingP/colors/xiaomi (3),/ProductImages/Acrylic360DegreeRotatingP/colors/xiaomi (4),/ProductImages/Acrylic360DegreeRotatingP/colors/xiaomi (5),/ProductImages/Acrylic360DegreeRotatingP/colors/xiaomi (6)</t>
+    </r>
+  </si>
+  <si>
+    <t>Xiaomi 5pro 12.4 2022</t>
   </si>
   <si>
     <r>
@@ -1125,11 +1151,22 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>273*210*14.0</t>
-    </r>
-  </si>
-  <si>
-    <t>Acrylic 414-Degree Rotating Protective Case</t>
+      <t>209*200*15.0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF1E4D78"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>/ProductImages/Acrylic360DegreeRotatingP/xiaomi (4)</t>
+    </r>
+  </si>
+  <si>
+    <t>Mi 6 2023</t>
   </si>
   <si>
     <r>
@@ -1139,146 +1176,18 @@
         <rFont val="CIDFont"/>
         <charset val="134"/>
       </rPr>
-      <t>Huawei Matepad Air 11.5 2023</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11.05"/>
-        <color rgb="FF000000"/>
-        <rFont val="CIDFont"/>
-        <charset val="134"/>
-      </rPr>
-      <t>265*194*13.0</t>
-    </r>
-  </si>
-  <si>
-    <t>Acrylic 415-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11.05"/>
-        <color rgb="FF000000"/>
-        <rFont val="CIDFont"/>
-        <charset val="134"/>
-      </rPr>
-      <t>TAB S9 11 2023</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11.05"/>
-        <color rgb="FF000000"/>
-        <rFont val="CIDFont"/>
-        <charset val="134"/>
-      </rPr>
-      <t>260*183*13.0</t>
-    </r>
-  </si>
-  <si>
-    <t>Acrylic 416-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11.05"/>
-        <color rgb="FF000000"/>
-        <rFont val="CIDFont"/>
-        <charset val="134"/>
-      </rPr>
-      <t>TAB S9FE 11 2023</t>
-    </r>
-  </si>
-  <si>
-    <t>Acrylic 417-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11.05"/>
-        <color rgb="FF000000"/>
-        <rFont val="CIDFont"/>
-        <charset val="134"/>
-      </rPr>
-      <t>TAB S9+ 12.4 2023</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11.05"/>
-        <color rgb="FF000000"/>
-        <rFont val="CIDFont"/>
-        <charset val="134"/>
-      </rPr>
-      <t>290*200*14.0</t>
-    </r>
-  </si>
-  <si>
-    <t>Acrylic 418-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11.05"/>
-        <color rgb="FF000000"/>
-        <rFont val="CIDFont"/>
-        <charset val="134"/>
-      </rPr>
-      <t>TAB S9+FE 12.4 2023</t>
-    </r>
-  </si>
-  <si>
-    <t>Acrylic 419-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11.05"/>
-        <color rgb="FF000000"/>
-        <rFont val="CIDFont"/>
-        <charset val="134"/>
-      </rPr>
-      <t>TAB A9 8.7 2023</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11.05"/>
-        <color rgb="FF000000"/>
-        <rFont val="CIDFont"/>
-        <charset val="134"/>
-      </rPr>
-      <t>215*140*11.0</t>
-    </r>
-  </si>
-  <si>
-    <t>Acrylic 420-Degree Rotating Protective Case</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11.05"/>
-        <color rgb="FF000000"/>
-        <rFont val="CIDFont"/>
-        <charset val="134"/>
-      </rPr>
-      <t>TAB A9+ 11 2023</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11.05"/>
-        <color rgb="FF000000"/>
-        <rFont val="CIDFont"/>
-        <charset val="134"/>
-      </rPr>
-      <t>260*185*14.0</t>
+      <t>260*181*13.7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color rgb="FF1E4D78"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>/ProductImages/Acrylic360DegreeRotatingP/xiaomi (5)</t>
     </r>
   </si>
 </sst>
@@ -1292,7 +1201,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="33">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1341,6 +1250,18 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF1E4D78"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
@@ -1838,137 +1759,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2003,6 +1924,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2540,8 +2467,8 @@
   <sheetPr/>
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -2561,50 +2488,50 @@
   </cols>
   <sheetData>
     <row r="1" ht="23.25" spans="1:16">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="11" t="s">
         <v>12</v>
       </c>
       <c r="D2" t="s">
@@ -3028,7 +2955,7 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -3048,50 +2975,50 @@
   </cols>
   <sheetData>
     <row r="1" ht="23.25" spans="1:16">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
     </row>
     <row r="2" customFormat="1" spans="1:10">
       <c r="A2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="11" t="s">
         <v>12</v>
       </c>
       <c r="D2" t="s">
@@ -3412,7 +3339,7 @@
       <c r="E14">
         <v>4.7</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="G14" s="11" t="s">
         <v>57</v>
       </c>
       <c r="H14">
@@ -3527,46 +3454,46 @@
   </cols>
   <sheetData>
     <row r="1" ht="23.25" spans="1:12">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="11"/>
+      <c r="L1" s="13"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="11" t="s">
         <v>12</v>
       </c>
       <c r="D2" t="s">
@@ -3815,7 +3742,7 @@
       <c r="E14">
         <v>4.7</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="G14" s="11" t="s">
         <v>60</v>
       </c>
       <c r="H14">
@@ -3884,7 +3811,7 @@
     </row>
     <row r="22" spans="2:4">
       <c r="B22" s="4"/>
-      <c r="D22" s="10"/>
+      <c r="D22" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3897,8 +3824,8 @@
   <sheetPr/>
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -3906,12 +3833,13 @@
     <col min="1" max="1" width="44.7142857142857" customWidth="1"/>
     <col min="2" max="2" width="28.1428571428571" customWidth="1"/>
     <col min="3" max="3" width="7.28571428571429" customWidth="1"/>
-    <col min="4" max="4" width="11.8571428571429" customWidth="1"/>
+    <col min="4" max="4" width="25.5714285714286" customWidth="1"/>
     <col min="5" max="5" width="17.7142857142857" customWidth="1"/>
     <col min="6" max="6" width="15.4285714285714" customWidth="1"/>
     <col min="7" max="7" width="15.8571428571429" customWidth="1"/>
     <col min="8" max="8" width="16.8571428571429" customWidth="1"/>
-    <col min="9" max="9" width="23.2857142857143" customWidth="1"/>
+    <col min="9" max="9" width="67.4285714285714" customWidth="1"/>
+    <col min="10" max="10" width="38" customWidth="1"/>
     <col min="11" max="11" width="25.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3960,20 +3888,24 @@
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
-        <v>74</v>
+        <v>13</v>
       </c>
       <c r="E2" s="4">
         <v>2.6</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H2" s="4">
         <v>235</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
+      <c r="I2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
@@ -3986,265 +3918,316 @@
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E3" s="4">
         <v>2.6</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H3" s="4">
         <v>235</v>
       </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
+      <c r="I3" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E4" s="4">
         <v>2.6</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H4" s="4">
         <v>240</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="I4" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E5" s="3">
         <v>2.8</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H5" s="4">
         <v>356</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+      <c r="I5" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B6" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E6" s="3">
         <v>2.8</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H6" s="4">
         <v>356</v>
       </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
+      <c r="I6" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="2" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B7" t="s">
         <v>23</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E7" s="3">
         <v>2.8</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H7" s="4">
         <v>356</v>
       </c>
-      <c r="J7" s="3"/>
+      <c r="I7" t="s">
+        <v>84</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="B8" t="s">
         <v>25</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E8" s="3">
         <v>2.8</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H8" s="4">
         <v>356</v>
       </c>
-      <c r="J8" s="3"/>
+      <c r="I8" t="s">
+        <v>85</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="2" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B9" t="s">
         <v>27</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E9" s="4">
         <v>2.8</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H9" s="4">
         <v>389</v>
       </c>
-      <c r="J9" s="3"/>
+      <c r="I9" t="s">
+        <v>87</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="2" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="B10" t="s">
         <v>30</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E10" s="4">
         <v>2.8</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H10" s="4">
         <v>389</v>
       </c>
-      <c r="J10" s="3"/>
+      <c r="I10" t="s">
+        <v>88</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="2" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="B11" t="s">
         <v>32</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E11" s="4">
         <v>2.8</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H11" s="4">
         <v>389</v>
       </c>
-      <c r="J11" s="3"/>
+      <c r="I11" t="s">
+        <v>89</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="2" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E12" s="4">
         <v>2.8</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H12" s="4">
         <v>388</v>
       </c>
-      <c r="J12" s="3"/>
+      <c r="I12" t="s">
+        <v>92</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="2" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E13" s="4">
         <v>2.8</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H13" s="4">
         <v>388</v>
       </c>
-      <c r="J13" s="3"/>
+      <c r="I13" t="s">
+        <v>75</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="2" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="B14" t="s">
         <v>38</v>
@@ -4261,19 +4244,24 @@
       <c r="H14" s="4">
         <v>391</v>
       </c>
-      <c r="J14" s="3"/>
+      <c r="I14" t="s">
+        <v>78</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="2" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="B15" t="s">
         <v>39</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E15" s="4">
         <v>2.8</v>
@@ -4284,19 +4272,24 @@
       <c r="H15" s="4">
         <v>391</v>
       </c>
-      <c r="J15" s="3"/>
+      <c r="I15" t="s">
+        <v>81</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="2" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="B16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E16" s="4">
         <v>2.8</v>
@@ -4307,19 +4300,24 @@
       <c r="H16" s="4">
         <v>391</v>
       </c>
-      <c r="J16" s="3"/>
+      <c r="I16" t="s">
+        <v>83</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="2" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="B17" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E17" s="4">
         <v>2.8</v>
@@ -4330,19 +4328,24 @@
       <c r="H17" s="4">
         <v>391</v>
       </c>
-      <c r="J17" s="3"/>
+      <c r="I17" t="s">
+        <v>84</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="2" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="B18" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E18" s="4">
         <v>2.8</v>
@@ -4353,19 +4356,24 @@
       <c r="H18" s="4">
         <v>391</v>
       </c>
-      <c r="J18" s="3"/>
+      <c r="I18" t="s">
+        <v>85</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="2" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="B19" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E19" s="4">
         <v>2.8</v>
@@ -4376,771 +4384,992 @@
       <c r="H19" s="4">
         <v>391</v>
       </c>
-      <c r="J19" s="3"/>
+      <c r="I19" t="s">
+        <v>92</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="2" t="s">
-        <v>104</v>
+        <v>72</v>
       </c>
       <c r="B20" t="s">
         <v>40</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E20" s="4">
         <v>4.2</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="H20" s="4">
         <v>429</v>
       </c>
-      <c r="J20" s="3"/>
+      <c r="I20" t="s">
+        <v>75</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="2" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
       <c r="B21" t="s">
         <v>42</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E21" s="4">
         <v>4.2</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="H21" s="4">
         <v>429</v>
       </c>
-      <c r="J21" s="3"/>
+      <c r="I21" t="s">
+        <v>78</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="2" t="s">
-        <v>107</v>
+        <v>72</v>
       </c>
       <c r="B22" t="s">
         <v>43</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E22" s="4">
         <v>4.2</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="H22" s="4">
         <v>429</v>
       </c>
-      <c r="J22" s="3"/>
+      <c r="I22" t="s">
+        <v>81</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="2" t="s">
-        <v>108</v>
+        <v>72</v>
       </c>
       <c r="B23" t="s">
         <v>44</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E23" s="4">
         <v>4.2</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="H23" s="4">
         <v>429</v>
       </c>
-      <c r="J23" s="3"/>
+      <c r="I23" t="s">
+        <v>83</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:10">
       <c r="A24" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H24" s="4">
+        <v>398</v>
+      </c>
+      <c r="I24" t="s">
+        <v>75</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D25" t="s">
+        <v>103</v>
+      </c>
+      <c r="E25" s="4">
+        <v>3.7</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H25" s="4">
+        <v>367</v>
+      </c>
+      <c r="I25" t="s">
+        <v>105</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="L25" s="3"/>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D26" t="s">
+        <v>103</v>
+      </c>
+      <c r="E26" s="4">
+        <v>4.9</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="H26" s="4">
+        <v>419</v>
+      </c>
+      <c r="I26" t="s">
+        <v>108</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B24" t="s">
+      <c r="D27" t="s">
         <v>110</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="E27" s="4">
+        <v>3.1</v>
+      </c>
+      <c r="G27" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="E24">
-        <v>3.7</v>
-      </c>
-      <c r="G24" t="s">
+      <c r="H27" s="4">
+        <v>356</v>
+      </c>
+      <c r="I27" t="s">
         <v>112</v>
       </c>
-      <c r="H24">
-        <v>374</v>
-      </c>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="2" t="s">
+      <c r="J27" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B25" t="s">
+      <c r="D28" t="s">
+        <v>110</v>
+      </c>
+      <c r="E28" s="4">
+        <v>3.1</v>
+      </c>
+      <c r="G28" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E25">
-        <v>3.7</v>
-      </c>
-      <c r="G25" t="s">
-        <v>112</v>
-      </c>
-      <c r="H25">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="2" t="s">
+      <c r="H28" s="4">
+        <v>379</v>
+      </c>
+      <c r="I28" t="s">
         <v>115</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="J28" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D29" t="s">
+        <v>110</v>
+      </c>
+      <c r="E29" s="4">
+        <v>3.1</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H29" s="4">
+        <v>379</v>
+      </c>
+      <c r="I29" t="s">
         <v>117</v>
       </c>
-      <c r="E26">
-        <v>3.7</v>
-      </c>
-      <c r="G26" s="4" t="s">
+      <c r="J29" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="H26" s="4">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="2" t="s">
+      <c r="D30" t="s">
+        <v>110</v>
+      </c>
+      <c r="E30" s="4">
+        <v>3.1</v>
+      </c>
+      <c r="G30" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="H30" s="4">
+        <v>372</v>
+      </c>
+      <c r="I30" t="s">
         <v>120</v>
       </c>
-      <c r="D27" t="s">
+      <c r="J30" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="E27">
-        <v>3.7</v>
-      </c>
-      <c r="G27" s="4" t="s">
+      <c r="D31" t="s">
+        <v>110</v>
+      </c>
+      <c r="E31" s="4">
+        <v>3.1</v>
+      </c>
+      <c r="G31" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="H27" s="4">
+      <c r="H31" s="4">
         <v>358</v>
       </c>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="2" t="s">
+      <c r="I31" t="s">
         <v>123</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="J31" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="D28" t="s">
-        <v>121</v>
-      </c>
-      <c r="E28">
-        <v>3.7</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="H28" s="4">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="D29" t="s">
-        <v>121</v>
-      </c>
-      <c r="E29" s="4">
-        <v>3.7</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="H29" s="4">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="D30" t="s">
-        <v>121</v>
-      </c>
-      <c r="E30" s="4">
-        <v>3.4</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="H30" s="4">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="D31" t="s">
-        <v>121</v>
-      </c>
-      <c r="E31" s="4">
-        <v>3.7</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="H31" s="4">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>135</v>
-      </c>
       <c r="D32" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="E32" s="4">
         <v>3.7</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="H32" s="4">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+        <v>379</v>
+      </c>
+      <c r="I32" t="s">
+        <v>125</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" s="2" t="s">
-        <v>137</v>
+        <v>72</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="D33" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="E33" s="4">
         <v>3.7</v>
       </c>
       <c r="G33" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="H33" s="4">
+        <v>334</v>
+      </c>
+      <c r="I33" t="s">
+        <v>128</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" ht="21" spans="1:10">
+      <c r="A34" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D34" t="s">
+        <v>130</v>
+      </c>
+      <c r="E34" s="4">
+        <v>3.4</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="H34" s="4">
+        <v>246</v>
+      </c>
+      <c r="I34" t="s">
+        <v>132</v>
+      </c>
+      <c r="J34" s="8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="35" ht="21" spans="1:10">
+      <c r="A35" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E35">
+        <v>3.7</v>
+      </c>
+      <c r="G35" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="H33">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="2" t="s">
+      <c r="H35" s="4">
+        <v>353</v>
+      </c>
+      <c r="I35" t="s">
+        <v>132</v>
+      </c>
+      <c r="J35" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="36" ht="21" spans="1:10">
+      <c r="A36" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D36" t="s">
         <v>139</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="E36" s="4">
+        <v>3.7</v>
+      </c>
+      <c r="G36" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="D34" t="s">
-        <v>121</v>
-      </c>
-      <c r="E34" s="4">
-        <v>4.9</v>
-      </c>
-      <c r="G34" s="4" t="s">
+      <c r="H36" s="4">
+        <v>363</v>
+      </c>
+      <c r="I36" t="s">
         <v>141</v>
       </c>
-      <c r="H34" s="4">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="2" t="s">
+      <c r="J36" s="8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="37" ht="21" spans="1:10">
+      <c r="A37" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="D37" t="s">
+        <v>139</v>
+      </c>
+      <c r="E37" s="4">
+        <v>3.4</v>
+      </c>
+      <c r="G37" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="D35" t="s">
-        <v>121</v>
-      </c>
-      <c r="E35" s="4">
-        <v>4.9</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="H35" s="4">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="2" t="s">
+      <c r="H37" s="4">
+        <v>234</v>
+      </c>
+      <c r="I37" t="s">
         <v>144</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="J37" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="38" ht="21" spans="1:10">
+      <c r="A38" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="D36" t="s">
-        <v>121</v>
-      </c>
-      <c r="E36" s="4">
-        <v>4.9</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="H36" s="4">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="2" t="s">
+      <c r="D38" t="s">
+        <v>139</v>
+      </c>
+      <c r="E38" s="4">
+        <v>3.7</v>
+      </c>
+      <c r="G38" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="H38" s="4">
+        <v>337</v>
+      </c>
+      <c r="I38" t="s">
+        <v>132</v>
+      </c>
+      <c r="J38" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="39" ht="21" spans="1:10">
+      <c r="A39" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B39" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="D37" t="s">
-        <v>121</v>
-      </c>
-      <c r="E37" s="4">
-        <v>5.6</v>
-      </c>
-      <c r="G37" s="4" t="s">
+      <c r="D39" t="s">
+        <v>139</v>
+      </c>
+      <c r="E39" s="4">
+        <v>3.7</v>
+      </c>
+      <c r="G39" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="H37" s="4">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="A38" s="2" t="s">
+      <c r="H39" s="4">
+        <v>335</v>
+      </c>
+      <c r="I39" t="s">
         <v>149</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="J39" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="40" ht="21" spans="1:10">
+      <c r="A40" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" s="4" t="s">
         <v>150</v>
-      </c>
-      <c r="D38" t="s">
-        <v>151</v>
-      </c>
-      <c r="E38" s="4">
-        <v>3.1</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="H38" s="4">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
-      <c r="A39" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="D39" t="s">
-        <v>151</v>
-      </c>
-      <c r="E39" s="4">
-        <v>3.1</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="H39" s="4">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
-      <c r="A40" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>157</v>
       </c>
       <c r="D40" t="s">
         <v>151</v>
       </c>
-      <c r="E40" s="4">
-        <v>3.1</v>
+      <c r="E40">
+        <v>3.7</v>
       </c>
       <c r="G40" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="H40" s="4">
+        <v>358</v>
+      </c>
+      <c r="I40" t="s">
+        <v>153</v>
+      </c>
+      <c r="J40" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="41" ht="21" spans="1:10">
+      <c r="A41" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="H40" s="4">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
-      <c r="A41" s="2" t="s">
+      <c r="D41" t="s">
+        <v>151</v>
+      </c>
+      <c r="E41">
+        <v>3.7</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="H41" s="4">
+        <v>336</v>
+      </c>
+      <c r="I41" t="s">
+        <v>157</v>
+      </c>
+      <c r="J41" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="42" ht="21" spans="1:10">
+      <c r="A42" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B42" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="B41" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="D41" t="s">
-        <v>160</v>
-      </c>
-      <c r="E41" s="4">
-        <v>3.7</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="H41" s="4">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
-      <c r="A42" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>163</v>
-      </c>
       <c r="D42" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="E42" s="4">
         <v>3.7</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="H42" s="4">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
+        <v>336</v>
+      </c>
+      <c r="I42" t="s">
+        <v>159</v>
+      </c>
+      <c r="J42" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="43" ht="21" spans="1:10">
       <c r="A43" s="2" t="s">
-        <v>166</v>
+        <v>72</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="D43" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="E43" s="4">
         <v>3.4</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="H43" s="4">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
+        <v>240</v>
+      </c>
+      <c r="I43" t="s">
+        <v>162</v>
+      </c>
+      <c r="J43" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="44" ht="21" spans="1:10">
       <c r="A44" s="2" t="s">
-        <v>170</v>
+        <v>72</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="D44" t="s">
         <v>151</v>
       </c>
       <c r="E44" s="4">
-        <v>3.1</v>
+        <v>3.7</v>
       </c>
       <c r="G44" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="H44" s="4">
+        <v>333</v>
+      </c>
+      <c r="I44" t="s">
+        <v>165</v>
+      </c>
+      <c r="J44" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="45" ht="21" spans="1:10">
+      <c r="A45" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D45" t="s">
+        <v>151</v>
+      </c>
+      <c r="E45" s="4">
+        <v>3.7</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="H45" s="4">
+        <v>371</v>
+      </c>
+      <c r="I45" t="s">
+        <v>168</v>
+      </c>
+      <c r="J45" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="46" ht="21" spans="1:10">
+      <c r="A46" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D46" t="s">
+        <v>151</v>
+      </c>
+      <c r="E46" s="4">
+        <v>3.7</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="H46">
+        <v>371</v>
+      </c>
+      <c r="I46" t="s">
+        <v>170</v>
+      </c>
+      <c r="J46" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="47" ht="21" spans="1:10">
+      <c r="A47" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="D47" t="s">
+        <v>151</v>
+      </c>
+      <c r="E47" s="4">
+        <v>4.9</v>
+      </c>
+      <c r="G47" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="H44" s="4">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="A45" s="2" t="s">
+      <c r="H47" s="4">
+        <v>460</v>
+      </c>
+      <c r="I47" t="s">
         <v>173</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="J47" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="48" ht="21" spans="1:10">
+      <c r="A48" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B48" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="D45" t="s">
-        <v>164</v>
-      </c>
-      <c r="E45" s="4">
-        <v>3.4</v>
-      </c>
-      <c r="G45" s="4" t="s">
+      <c r="D48" t="s">
+        <v>151</v>
+      </c>
+      <c r="E48" s="4">
+        <v>4.9</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="H48" s="4">
+        <v>460</v>
+      </c>
+      <c r="I48" t="s">
         <v>175</v>
       </c>
-      <c r="H45" s="4">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="A46" s="2" t="s">
+      <c r="J48" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="49" ht="21" spans="1:10">
+      <c r="A49" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B49" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="B46" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="D46" t="s">
-        <v>121</v>
-      </c>
-      <c r="E46" s="4">
-        <v>3.4</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="H46" s="4">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
-      <c r="A47" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="D47" t="s">
-        <v>164</v>
-      </c>
-      <c r="E47" s="4">
-        <v>3.7</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="H47" s="4">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
-      <c r="A48" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="D48" t="s">
-        <v>184</v>
-      </c>
-      <c r="E48" s="4">
-        <v>3.7</v>
-      </c>
-      <c r="G48" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="H48" s="4">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8">
-      <c r="A49" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>186</v>
-      </c>
       <c r="D49" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="E49" s="4">
         <v>4.9</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="H49" s="4">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8">
+        <v>460</v>
+      </c>
+      <c r="I49" t="s">
+        <v>177</v>
+      </c>
+      <c r="J49" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="50" ht="21" spans="1:10">
       <c r="A50" s="2" t="s">
-        <v>188</v>
+        <v>72</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="D50" t="s">
         <v>151</v>
       </c>
       <c r="E50" s="4">
-        <v>3.1</v>
+        <v>5.6</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="H50" s="4">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8">
+        <v>563</v>
+      </c>
+      <c r="I50" t="s">
+        <v>153</v>
+      </c>
+      <c r="J50" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="51" ht="21" spans="1:10">
       <c r="A51" s="2" t="s">
-        <v>191</v>
+        <v>72</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="D51" t="s">
-        <v>111</v>
+        <v>151</v>
       </c>
       <c r="E51" s="4">
-        <v>4.9</v>
+        <v>3.4</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="H51" s="4">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8">
+        <v>234</v>
+      </c>
+      <c r="I51" t="s">
+        <v>157</v>
+      </c>
+      <c r="J51" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="52" ht="21" spans="1:10">
       <c r="A52" s="2" t="s">
-        <v>194</v>
+        <v>72</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="D52" t="s">
-        <v>13</v>
+        <v>151</v>
       </c>
       <c r="E52" s="4">
-        <v>2.8</v>
+        <v>3.7</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="H52" s="4">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8">
+        <v>303</v>
+      </c>
+      <c r="I52" t="s">
+        <v>159</v>
+      </c>
+      <c r="J52" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="53" ht="21" spans="1:10">
       <c r="A53" s="2" t="s">
-        <v>197</v>
+        <v>72</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="D53" t="s">
-        <v>111</v>
+        <v>151</v>
       </c>
       <c r="E53" s="4">
         <v>3.7</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="H53" s="4">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8">
+        <v>303</v>
+      </c>
+      <c r="I53" t="s">
+        <v>162</v>
+      </c>
+      <c r="J53" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="54" ht="21" spans="1:10">
       <c r="A54" s="2" t="s">
-        <v>200</v>
+        <v>72</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="D54" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="E54" s="4">
-        <v>3.7</v>
+        <v>4.2</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="H54" s="4">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8">
+        <v>369</v>
+      </c>
+      <c r="I54" t="s">
+        <v>153</v>
+      </c>
+      <c r="J54" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="55" ht="21" spans="1:10">
       <c r="A55" s="2" t="s">
-        <v>203</v>
+        <v>72</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
       <c r="D55" t="s">
         <v>151</v>
       </c>
       <c r="E55" s="4">
-        <v>3.7</v>
+        <v>4.2</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>155</v>
+        <v>186</v>
       </c>
       <c r="H55" s="4">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8">
+        <v>369</v>
+      </c>
+      <c r="I55" t="s">
+        <v>157</v>
+      </c>
+      <c r="J55" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="56" ht="21" spans="1:10">
       <c r="A56" s="2" t="s">
-        <v>205</v>
+        <v>72</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>206</v>
+        <v>188</v>
       </c>
       <c r="D56" t="s">
-        <v>184</v>
+        <v>151</v>
       </c>
       <c r="E56" s="4">
-        <v>4.2</v>
+        <v>3.1</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
       <c r="H56" s="4">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8">
+        <v>200</v>
+      </c>
+      <c r="I56" t="s">
+        <v>159</v>
+      </c>
+      <c r="J56" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="57" ht="21" spans="1:10">
       <c r="A57" s="2" t="s">
-        <v>208</v>
+        <v>72</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
       <c r="D57" t="s">
         <v>151</v>
@@ -5149,133 +5378,179 @@
         <v>3.7</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>210</v>
+        <v>191</v>
       </c>
       <c r="H57" s="4">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8">
+        <v>310</v>
+      </c>
+      <c r="I57" t="s">
+        <v>162</v>
+      </c>
+      <c r="J57" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="58" ht="21" spans="1:10">
       <c r="A58" s="2" t="s">
-        <v>211</v>
+        <v>72</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="D58" t="s">
-        <v>121</v>
+        <v>193</v>
       </c>
       <c r="E58" s="4">
         <v>3.7</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>213</v>
+        <v>140</v>
       </c>
       <c r="H58" s="4">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8">
+        <v>363</v>
+      </c>
+      <c r="I58" t="s">
+        <v>153</v>
+      </c>
+      <c r="J58" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="59" ht="21" spans="1:10">
       <c r="A59" s="2" t="s">
-        <v>214</v>
+        <v>72</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>215</v>
+        <v>194</v>
       </c>
       <c r="D59" t="s">
-        <v>121</v>
+        <v>193</v>
       </c>
       <c r="E59" s="4">
+        <v>4.2</v>
+      </c>
+      <c r="G59" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="H59" s="4">
+        <v>353</v>
+      </c>
+      <c r="I59" t="s">
+        <v>159</v>
+      </c>
+      <c r="J59" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="60" ht="21" spans="1:11">
+      <c r="A60" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B60" t="s">
+        <v>196</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="E60">
         <v>3.7</v>
       </c>
-      <c r="G59" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="H59" s="4">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8">
-      <c r="A60" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="D60" t="s">
-        <v>121</v>
-      </c>
-      <c r="E60" s="4">
-        <v>4.2</v>
-      </c>
-      <c r="G60" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="H60" s="4">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8">
+      <c r="G60" t="s">
+        <v>198</v>
+      </c>
+      <c r="H60">
+        <v>374</v>
+      </c>
+      <c r="I60" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="J60" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="K60" s="3"/>
+    </row>
+    <row r="61" ht="21" spans="1:10">
       <c r="A61" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="D61" t="s">
-        <v>121</v>
-      </c>
-      <c r="E61" s="4">
-        <v>4.2</v>
-      </c>
-      <c r="G61" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="H61" s="4">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8">
+        <v>72</v>
+      </c>
+      <c r="B61" t="s">
+        <v>201</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="E61">
+        <v>3.7</v>
+      </c>
+      <c r="G61" t="s">
+        <v>198</v>
+      </c>
+      <c r="H61">
+        <v>374</v>
+      </c>
+      <c r="I61" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="J61" s="9" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="62" ht="21" spans="1:10">
       <c r="A62" s="2" t="s">
-        <v>221</v>
+        <v>72</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
       <c r="D62" t="s">
-        <v>121</v>
+        <v>197</v>
       </c>
       <c r="E62" s="4">
-        <v>3.1</v>
+        <v>4.9</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="H62" s="4">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8">
+        <v>459</v>
+      </c>
+      <c r="I62" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="J62" s="9" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="63" ht="21" spans="1:10">
       <c r="A63" s="2" t="s">
-        <v>224</v>
+        <v>72</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="D63" t="s">
-        <v>121</v>
+        <v>197</v>
       </c>
       <c r="E63" s="4">
         <v>3.7</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
       <c r="H63" s="4">
-        <v>310</v>
+        <v>305</v>
+      </c>
+      <c r="I63" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="J63" s="9" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:K63">
+    <sortCondition ref="D2:D63"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
upto skin like back sticker solid co product uploaded
</commit_message>
<xml_diff>
--- a/ChaoKaiQiProducts.xlsx
+++ b/ChaoKaiQiProducts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12210" firstSheet="8" activeTab="12"/>
+    <workbookView windowWidth="28800" windowHeight="12210" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Snap rotate style" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Acrylic 360-Degree Rotating P" sheetId="5" r:id="rId4"/>
     <sheet name="Acrylic Two-in-One magnetic" sheetId="6" r:id="rId5"/>
     <sheet name="AcrylicTwo-in-OneIntegratedS" sheetId="7" r:id="rId6"/>
-    <sheet name="Acrylic Two-in-One Y Fold Side " sheetId="8" r:id="rId7"/>
+    <sheet name="Acrylic Two-in-One Y Fold Side" sheetId="8" r:id="rId7"/>
     <sheet name="Skin-like Back Sticker Solid Co" sheetId="9" r:id="rId8"/>
     <sheet name="Painted Back Sticker Solid Colo" sheetId="10" r:id="rId9"/>
     <sheet name="Snowflake Pattern Anti-drop Tra" sheetId="11" r:id="rId10"/>
@@ -7131,7 +7131,7 @@
   <sheetPr/>
   <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
@@ -13707,8 +13707,8 @@
   <sheetPr/>
   <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView topLeftCell="B30" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -13768,7 +13768,7 @@
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="E2" s="2">
         <v>2.6</v>
@@ -15472,8 +15472,8 @@
   <sheetPr/>
   <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>

</xml_diff>